<commit_message>
Add Alexis chocho -.-
</commit_message>
<xml_diff>
--- a/src/assets/data/BD_INVITADOS.xlsx
+++ b/src/assets/data/BD_INVITADOS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccloz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Claudia Documentos\CYB\proyectos\angular\AppWedding\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650DA23D-D619-4E6F-844F-C7BB24A443C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21165CD-B972-4796-9FD3-9026848767AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="120">
   <si>
     <t>invitado</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>Tío Antonio Fernández Marrufo</t>
+  </si>
+  <si>
+    <t>Alexis Maldonado Vásquez</t>
+  </si>
+  <si>
+    <t>BC0000053</t>
   </si>
 </sst>
 </file>
@@ -772,11 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +827,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -857,12 +862,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C9" si="0">CONCATENATE(E3,F3)</f>
@@ -892,7 +897,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -927,7 +932,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -962,7 +967,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1032,7 +1037,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1067,7 +1072,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1102,7 +1107,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1137,7 +1142,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1172,7 +1177,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1207,7 +1212,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1242,7 +1247,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1282,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1312,7 +1317,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1382,7 +1387,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1417,7 +1422,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1452,7 +1457,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1487,7 +1492,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1522,7 +1527,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1557,7 +1562,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1592,7 +1597,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2187,7 +2192,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -2222,7 +2227,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -2257,7 +2262,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -2292,7 +2297,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2327,7 +2332,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -2362,7 +2367,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -2397,7 +2402,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -2432,7 +2437,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -2467,7 +2472,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -2502,7 +2507,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -2537,7 +2542,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -2572,7 +2577,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -2607,7 +2612,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -2642,26 +2647,51 @@
         <v>116</v>
       </c>
     </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" ref="C54" si="4">CONCATENATE(E54,F54)</f>
+        <v>BC000005387126</v>
+      </c>
+      <c r="D54">
+        <v>968238265</v>
+      </c>
+      <c r="E54" t="s">
+        <v>119</v>
+      </c>
+      <c r="F54">
+        <f>Hoja2!B54</f>
+        <v>87126</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" ref="H54" si="5">CONCATENATE(G54,C54)</f>
+        <v>https://bvasquez-code.github.io/AppWedding/?id=BC000005387126</v>
+      </c>
+      <c r="I54" t="s">
+        <v>113</v>
+      </c>
+      <c r="J54" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J53" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Braulio"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Familia"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{13788AC9-6D19-49A5-9426-2415D075C294}"/>
     <hyperlink ref="G3:G53" r:id="rId2" display="https://bvasquez-code.github.io/AppWedding/?id=" xr:uid="{D11B3EBB-EBFB-4F3F-9B0C-7B65325CA175}"/>
+    <hyperlink ref="G54" r:id="rId3" xr:uid="{2E0D1352-D939-471C-AD35-0E844912A9E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -5394,1801 +5424,1801 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*100000</f>
-        <v>38120.079273117168</v>
+        <v>90736.860033971199</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A65" ca="1" si="0">RAND()*100000</f>
-        <v>36897.436302618014</v>
+        <v>2503.8012780059239</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>60213.293167504089</v>
+        <v>83118.351738091122</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>2824.6128826877602</v>
+        <v>9337.9864854793432</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>36664.128333152759</v>
+        <v>60575.81080335813</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>86762.408971744735</v>
+        <v>83365.633348564254</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>44694.012436518096</v>
+        <v>62648.281861040952</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>24765.741408945672</v>
+        <v>41470.568991551649</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>95549.257300080091</v>
+        <v>47715.944672102298</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>70442.134516866179</v>
+        <v>775.90278926115138</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>84729.907959296659</v>
+        <v>72258.437013518604</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>17402.968106162509</v>
+        <v>61155.55662353697</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>78775.241952876546</v>
+        <v>36223.096133193489</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>55160.351367313917</v>
+        <v>31751.156397744275</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>35552.686936037237</v>
+        <v>32301.752060134149</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>36591.440562676195</v>
+        <v>3094.3110719305332</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>4634.3679680050709</v>
+        <v>23381.876534606617</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>70936.575244334861</v>
+        <v>91151.537542923295</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f ca="1">RAND()*100000</f>
-        <v>1970.2755614332102</v>
+        <v>20499.243401657553</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>59061.586830273824</v>
+        <v>25511.11942172244</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>40346.480059090063</v>
+        <v>86810.714742376673</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>88073.807392124843</v>
+        <v>33086.421342993111</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>7520.1182460078235</v>
+        <v>31898.126775060264</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>71549.586339113463</v>
+        <v>46251.289426291441</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>31982.478772186307</v>
+        <v>98567.246015143945</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>77619.404058259257</v>
+        <v>75745.680001250643</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>956.12831882407875</v>
+        <v>77879.019956473203</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>31813.541815514069</v>
+        <v>97941.653442177907</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>59721.866164567495</v>
+        <v>64322.26819359287</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>59822.79130976017</v>
+        <v>11928.515757656443</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>80523.463741624873</v>
+        <v>52095.412220635451</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>18596.934941463471</v>
+        <v>43488.166253795527</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>24032.09283836991</v>
+        <v>69733.376332985485</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>78178.992995280612</v>
+        <v>40724.253090965947</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>68322.447830077697</v>
+        <v>73733.550788772292</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>23714.939728447771</v>
+        <v>86049.752397571239</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>75713.715240115373</v>
+        <v>32414.982809795125</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>57908.510718691345</v>
+        <v>93121.815205855193</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>20618.545090889384</v>
+        <v>22342.315567976857</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>61855.113841227372</v>
+        <v>91012.798249258311</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>92652.804919693954</v>
+        <v>8769.7523532735522</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>20014.488050089298</v>
+        <v>35516.003024586462</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>60657.284885355708</v>
+        <v>64276.287733256097</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>31033.462138436396</v>
+        <v>29144.609499746875</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>24244.874965835272</v>
+        <v>88195.892734006586</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>61316.394710075903</v>
+        <v>72187.51388134736</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>96225.781211156151</v>
+        <v>29924.088588850162</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>97549.794764292586</v>
+        <v>94310.872553092078</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>23052.123106557952</v>
+        <v>32506.760631131227</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>10658.772541089911</v>
+        <v>49505.456628064567</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>72399.141502919767</v>
+        <v>82487.117973839981</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>68429.527105745074</v>
+        <v>10923.972248296854</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>75066.525523734075</v>
+        <v>23339.585870572409</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>77281.388169108381</v>
+        <v>14862.765779725429</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>34403.100739087022</v>
+        <v>83332.522216968864</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>47381.373574633304</v>
+        <v>21594.168821377323</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>89175.072855311213</v>
+        <v>77107.558884849874</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>47218.3815507037</v>
+        <v>10301.757356551321</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>35075.932757587965</v>
+        <v>60332.672585823253</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>93188.003531166803</v>
+        <v>15585.755577295156</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>77481.38947655134</v>
+        <v>6455.9564120985624</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>62826.410406642863</v>
+        <v>98901.979418193878</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>64080.293218419385</v>
+        <v>68848.215303188204</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>29091.142313852124</v>
+        <v>83774.754406866981</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" ca="1" si="0"/>
-        <v>69567.59502407597</v>
+        <v>2897.4399100831215</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" ref="A66:A129" ca="1" si="1">RAND()*100000</f>
-        <v>11245.537265121753</v>
+        <v>78438.678425546939</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ca="1" si="1"/>
-        <v>76195.416912140572</v>
+        <v>99861.678863374153</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ca="1" si="1"/>
-        <v>87303.054939132213</v>
+        <v>6318.6718159558786</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" ca="1" si="1"/>
-        <v>9189.3793221451851</v>
+        <v>85932.703174499402</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" ca="1" si="1"/>
-        <v>67029.655816549464</v>
+        <v>34479.52663072975</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" ca="1" si="1"/>
-        <v>12448.490471139461</v>
+        <v>16464.335890213322</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" ca="1" si="1"/>
-        <v>91051.664887151535</v>
+        <v>76170.365756500774</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" ca="1" si="1"/>
-        <v>17612.746239822096</v>
+        <v>35245.469263806648</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" ca="1" si="1"/>
-        <v>85526.679708007432</v>
+        <v>15074.330284963811</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" ca="1" si="1"/>
-        <v>28287.978756720677</v>
+        <v>5393.9314205522669</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" ca="1" si="1"/>
-        <v>69909.625655300493</v>
+        <v>25736.877030210671</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" ca="1" si="1"/>
-        <v>18018.983197042005</v>
+        <v>89112.12085053316</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" ca="1" si="1"/>
-        <v>94374.547027590146</v>
+        <v>64914.558864445935</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" ca="1" si="1"/>
-        <v>19302.746721448784</v>
+        <v>67420.226584212272</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" ca="1" si="1"/>
-        <v>16657.376881970398</v>
+        <v>14669.918883861377</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" ca="1" si="1"/>
-        <v>79413.617248026887</v>
+        <v>48390.735861757406</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" ca="1" si="1"/>
-        <v>64520.471641047217</v>
+        <v>31383.465903492204</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" ca="1" si="1"/>
-        <v>7213.5764470186768</v>
+        <v>21380.198105787917</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" ca="1" si="1"/>
-        <v>33535.252914518111</v>
+        <v>74427.696590101317</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" ca="1" si="1"/>
-        <v>99353.455080543979</v>
+        <v>4009.5391804007563</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" ca="1" si="1"/>
-        <v>38766.299189765799</v>
+        <v>5601.3396858580418</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" ca="1" si="1"/>
-        <v>42939.766543261772</v>
+        <v>88073.593668359827</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" ca="1" si="1"/>
-        <v>57154.605982288245</v>
+        <v>34401.320740336152</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" ca="1" si="1"/>
-        <v>80732.10688521502</v>
+        <v>71795.369540918808</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" ca="1" si="1"/>
-        <v>42519.791796592297</v>
+        <v>12199.795050675299</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" ca="1" si="1"/>
-        <v>3330.9838613992615</v>
+        <v>20193.814578480706</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" ca="1" si="1"/>
-        <v>43629.354597202517</v>
+        <v>21811.544050686203</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" ca="1" si="1"/>
-        <v>75626.577595923882</v>
+        <v>36173.637729452603</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" ca="1" si="1"/>
-        <v>55588.114212167136</v>
+        <v>74894.794649724208</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" ca="1" si="1"/>
-        <v>81562.385021283611</v>
+        <v>86230.975923387945</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" ca="1" si="1"/>
-        <v>52733.608815995438</v>
+        <v>27930.6716837163</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" ca="1" si="1"/>
-        <v>99182.99390440312</v>
+        <v>48886.863804330147</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" ca="1" si="1"/>
-        <v>7226.7256290546648</v>
+        <v>57209.307107347871</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" ca="1" si="1"/>
-        <v>31673.272253101935</v>
+        <v>29954.171973717701</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" ca="1" si="1"/>
-        <v>3921.207554094497</v>
+        <v>79793.409423418343</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" ca="1" si="1"/>
-        <v>3793.656294501724</v>
+        <v>90316.067698339291</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" ca="1" si="1"/>
-        <v>78901.712340357451</v>
+        <v>25034.000936731292</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" ca="1" si="1"/>
-        <v>21437.188205068614</v>
+        <v>28843.090808524696</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" ca="1" si="1"/>
-        <v>17833.330367486687</v>
+        <v>35237.528769875724</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" ca="1" si="1"/>
-        <v>75560.6333703977</v>
+        <v>20422.708790197041</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" ca="1" si="1"/>
-        <v>5011.1949766764028</v>
+        <v>79901.952483807341</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" ca="1" si="1"/>
-        <v>59701.786377652556</v>
+        <v>46985.98765983757</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" ca="1" si="1"/>
-        <v>71113.589270104101</v>
+        <v>89141.990021874779</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" ca="1" si="1"/>
-        <v>88132.411523106784</v>
+        <v>2287.8075046803283</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" ca="1" si="1"/>
-        <v>6163.9095547515235</v>
+        <v>53637.946481309671</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" ca="1" si="1"/>
-        <v>13495.123101696905</v>
+        <v>91556.238241418992</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" ca="1" si="1"/>
-        <v>35369.519501624782</v>
+        <v>2847.1606511998202</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" ca="1" si="1"/>
-        <v>64663.408283869219</v>
+        <v>25600.711771817209</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" ca="1" si="1"/>
-        <v>96431.622323824791</v>
+        <v>2170.8783392761056</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" ca="1" si="1"/>
-        <v>30064.165890020755</v>
+        <v>23172.580568463753</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" ca="1" si="1"/>
-        <v>69813.801015122284</v>
+        <v>73827.591523284835</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" ca="1" si="1"/>
-        <v>16143.492170760343</v>
+        <v>23102.134828154609</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" ca="1" si="1"/>
-        <v>96711.66966095363</v>
+        <v>33541.630201496395</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" ca="1" si="1"/>
-        <v>5754.9058045426982</v>
+        <v>35601.884466780641</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" ca="1" si="1"/>
-        <v>97439.458903661347</v>
+        <v>5528.6872369361809</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" ca="1" si="1"/>
-        <v>698.76040967299377</v>
+        <v>14714.529861269664</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" ca="1" si="1"/>
-        <v>47085.749570309184</v>
+        <v>21251.048971037912</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" ca="1" si="1"/>
-        <v>6718.6253287439768</v>
+        <v>90579.216427302832</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" ca="1" si="1"/>
-        <v>32342.428673217062</v>
+        <v>62547.540757594164</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" ca="1" si="1"/>
-        <v>27009.252156986939</v>
+        <v>493.53992509139078</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" ca="1" si="1"/>
-        <v>44285.184927479328</v>
+        <v>37634.676485357973</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" ca="1" si="1"/>
-        <v>42817.920861757229</v>
+        <v>30259.029954207839</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" ca="1" si="1"/>
-        <v>78088.539362062395</v>
+        <v>91225.259627760621</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" ca="1" si="1"/>
-        <v>17475.140648950626</v>
+        <v>17740.510554417564</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" ref="A130:A193" ca="1" si="2">RAND()*100000</f>
-        <v>64589.016883326585</v>
+        <v>20278.492139505201</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" ca="1" si="2"/>
-        <v>70706.509822371212</v>
+        <v>20624.796747132725</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" ca="1" si="2"/>
-        <v>92742.171323688599</v>
+        <v>23166.437994524404</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" ca="1" si="2"/>
-        <v>44851.992615979951</v>
+        <v>74676.819068800847</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" ca="1" si="2"/>
-        <v>35007.98056188503</v>
+        <v>14266.288309148744</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
         <f t="shared" ca="1" si="2"/>
-        <v>28040.387464816729</v>
+        <v>85581.104374570408</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
         <f t="shared" ca="1" si="2"/>
-        <v>11612.17428074437</v>
+        <v>84135.038064638473</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
         <f t="shared" ca="1" si="2"/>
-        <v>21836.373873246663</v>
+        <v>22602.778082316167</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
         <f t="shared" ca="1" si="2"/>
-        <v>92496.693823826368</v>
+        <v>52188.393760384773</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
         <f t="shared" ca="1" si="2"/>
-        <v>8673.3737047975046</v>
+        <v>71469.431805900007</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
         <f t="shared" ca="1" si="2"/>
-        <v>96580.181763415763</v>
+        <v>52820.887272854256</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
         <f t="shared" ca="1" si="2"/>
-        <v>71570.225636071409</v>
+        <v>5818.7572850221577</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
         <f t="shared" ca="1" si="2"/>
-        <v>59408.419873383333</v>
+        <v>82382.900070252712</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
         <f t="shared" ca="1" si="2"/>
-        <v>60119.960481871058</v>
+        <v>77822.120921208101</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
         <f t="shared" ca="1" si="2"/>
-        <v>7517.2636636541056</v>
+        <v>77720.740018211422</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
         <f t="shared" ca="1" si="2"/>
-        <v>47165.617996755915</v>
+        <v>67330.623984737133</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
         <f t="shared" ca="1" si="2"/>
-        <v>14049.219622256103</v>
+        <v>25591.080188875192</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
         <f t="shared" ca="1" si="2"/>
-        <v>91844.34635158263</v>
+        <v>56477.826709065768</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
         <f t="shared" ca="1" si="2"/>
-        <v>68723.518201665051</v>
+        <v>30485.846102638581</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
         <f t="shared" ca="1" si="2"/>
-        <v>34922.282741028474</v>
+        <v>29282.888295383193</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
         <f t="shared" ca="1" si="2"/>
-        <v>40022.490110940467</v>
+        <v>95212.534168385639</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
         <f t="shared" ca="1" si="2"/>
-        <v>50038.240577576711</v>
+        <v>86910.875828342367</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
         <f t="shared" ca="1" si="2"/>
-        <v>91893.568492044011</v>
+        <v>57702.672000187697</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153">
         <f t="shared" ca="1" si="2"/>
-        <v>59936.638771609418</v>
+        <v>6022.2908745765972</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154">
         <f t="shared" ca="1" si="2"/>
-        <v>92182.522699167617</v>
+        <v>53914.97046772029</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155">
         <f t="shared" ca="1" si="2"/>
-        <v>37956.978222061858</v>
+        <v>76007.354464375807</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156">
         <f t="shared" ca="1" si="2"/>
-        <v>36165.974964035893</v>
+        <v>50177.716420648823</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157">
         <f t="shared" ca="1" si="2"/>
-        <v>23723.848626279898</v>
+        <v>8683.8751395375002</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158">
         <f t="shared" ca="1" si="2"/>
-        <v>59602.236926222999</v>
+        <v>31393.062222877856</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159">
         <f t="shared" ca="1" si="2"/>
-        <v>9939.8165028463445</v>
+        <v>27831.320592099572</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160">
         <f t="shared" ca="1" si="2"/>
-        <v>45387.592981800437</v>
+        <v>73028.194082651593</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161">
         <f t="shared" ca="1" si="2"/>
-        <v>8347.6618126845042</v>
+        <v>3772.0854462896746</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162">
         <f t="shared" ca="1" si="2"/>
-        <v>13659.127291848083</v>
+        <v>20975.317552304918</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163">
         <f t="shared" ca="1" si="2"/>
-        <v>43082.40001823708</v>
+        <v>42738.895941626601</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164">
         <f t="shared" ca="1" si="2"/>
-        <v>92534.372984333706</v>
+        <v>74617.684583386697</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165">
         <f t="shared" ca="1" si="2"/>
-        <v>42413.080793636145</v>
+        <v>62996.799073690956</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166">
         <f t="shared" ca="1" si="2"/>
-        <v>19509.527295082207</v>
+        <v>26214.552020151616</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167">
         <f t="shared" ca="1" si="2"/>
-        <v>7629.7696310262509</v>
+        <v>12454.757760697266</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168">
         <f t="shared" ca="1" si="2"/>
-        <v>68354.377805375072</v>
+        <v>28592.467988828619</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169">
         <f t="shared" ca="1" si="2"/>
-        <v>56385.983365880442</v>
+        <v>56801.193137073693</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170">
         <f t="shared" ca="1" si="2"/>
-        <v>52309.081229092291</v>
+        <v>3805.833594751995</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171">
         <f t="shared" ca="1" si="2"/>
-        <v>39319.237222178446</v>
+        <v>75349.638014740442</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172">
         <f t="shared" ca="1" si="2"/>
-        <v>97114.475288538742</v>
+        <v>56927.124301647666</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173">
         <f t="shared" ca="1" si="2"/>
-        <v>12123.766249216105</v>
+        <v>66065.3758292087</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174">
         <f t="shared" ca="1" si="2"/>
-        <v>7645.5068585010386</v>
+        <v>88244.17135242738</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175">
         <f t="shared" ca="1" si="2"/>
-        <v>28554.407125331614</v>
+        <v>9894.7036929901587</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176">
         <f t="shared" ca="1" si="2"/>
-        <v>39114.882979208734</v>
+        <v>59072.014020463444</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177">
         <f t="shared" ca="1" si="2"/>
-        <v>54950.516297119015</v>
+        <v>97691.926073731578</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178">
         <f t="shared" ca="1" si="2"/>
-        <v>35648.069382576643</v>
+        <v>28585.165871896847</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179">
         <f t="shared" ca="1" si="2"/>
-        <v>58784.705756710253</v>
+        <v>49691.544516833586</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180">
         <f t="shared" ca="1" si="2"/>
-        <v>74161.453204294623</v>
+        <v>66452.706803833542</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181">
         <f t="shared" ca="1" si="2"/>
-        <v>6174.856745112811</v>
+        <v>82949.163624176086</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182">
         <f t="shared" ca="1" si="2"/>
-        <v>93474.230898349386</v>
+        <v>74097.428877572485</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183">
         <f t="shared" ca="1" si="2"/>
-        <v>58002.001359074842</v>
+        <v>33205.926709682979</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184">
         <f t="shared" ca="1" si="2"/>
-        <v>81412.594831006922</v>
+        <v>64743.787255370677</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185">
         <f t="shared" ca="1" si="2"/>
-        <v>3146.1016405764708</v>
+        <v>85961.089642749153</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186">
         <f t="shared" ca="1" si="2"/>
-        <v>35711.282249293188</v>
+        <v>22305.940779839417</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187">
         <f t="shared" ca="1" si="2"/>
-        <v>34415.584645195398</v>
+        <v>74324.347323886861</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188">
         <f t="shared" ca="1" si="2"/>
-        <v>21328.232154184479</v>
+        <v>42877.396543667492</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189">
         <f t="shared" ca="1" si="2"/>
-        <v>13550.512929067914</v>
+        <v>25554.212323545533</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190">
         <f t="shared" ca="1" si="2"/>
-        <v>5053.3248223798564</v>
+        <v>13517.569446655953</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191">
         <f t="shared" ca="1" si="2"/>
-        <v>29912.376676876007</v>
+        <v>81323.801653193397</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192">
         <f t="shared" ca="1" si="2"/>
-        <v>66828.904093004676</v>
+        <v>79379.861063278964</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193">
         <f t="shared" ca="1" si="2"/>
-        <v>85586.049653920709</v>
+        <v>91722.389917640437</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194">
         <f t="shared" ref="A194:A257" ca="1" si="3">RAND()*100000</f>
-        <v>91628.026927061917</v>
+        <v>95224.07559382476</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195">
         <f t="shared" ca="1" si="3"/>
-        <v>19048.518392975366</v>
+        <v>86732.334906064629</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196">
         <f t="shared" ca="1" si="3"/>
-        <v>81412.418757596432</v>
+        <v>86005.974642585934</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197">
         <f t="shared" ca="1" si="3"/>
-        <v>56020.791814022065</v>
+        <v>24880.523421107082</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198">
         <f t="shared" ca="1" si="3"/>
-        <v>88356.746521541907</v>
+        <v>78416.346673341104</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199">
         <f t="shared" ca="1" si="3"/>
-        <v>76329.433437974032</v>
+        <v>80631.669705524357</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200">
         <f t="shared" ca="1" si="3"/>
-        <v>28516.813500924854</v>
+        <v>92630.356228096323</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201">
         <f t="shared" ca="1" si="3"/>
-        <v>96359.169043628397</v>
+        <v>1519.8164219514365</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202">
         <f t="shared" ca="1" si="3"/>
-        <v>3753.9035594990169</v>
+        <v>27530.738498697981</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203">
         <f t="shared" ca="1" si="3"/>
-        <v>26393.037249611563</v>
+        <v>54880.619822162938</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204">
         <f t="shared" ca="1" si="3"/>
-        <v>6270.4505898789175</v>
+        <v>97896.674501906091</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205">
         <f t="shared" ca="1" si="3"/>
-        <v>4853.7896768126029</v>
+        <v>61428.491653964848</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206">
         <f t="shared" ca="1" si="3"/>
-        <v>30658.407735704262</v>
+        <v>75699.809362095577</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207">
         <f t="shared" ca="1" si="3"/>
-        <v>48174.014339270208</v>
+        <v>38539.200212812619</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208">
         <f t="shared" ca="1" si="3"/>
-        <v>23203.11710986208</v>
+        <v>78571.482284541999</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209">
         <f t="shared" ca="1" si="3"/>
-        <v>89241.870707348688</v>
+        <v>56996.227688696388</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210">
         <f t="shared" ca="1" si="3"/>
-        <v>72955.812015559117</v>
+        <v>92875.15265278492</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211">
         <f t="shared" ca="1" si="3"/>
-        <v>46492.767020112202</v>
+        <v>27648.792867251803</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212">
         <f t="shared" ca="1" si="3"/>
-        <v>66211.242711101353</v>
+        <v>45902.267122974074</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213">
         <f t="shared" ca="1" si="3"/>
-        <v>55864.674072402784</v>
+        <v>94158.551129644839</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214">
         <f t="shared" ca="1" si="3"/>
-        <v>95913.767342088162</v>
+        <v>15337.461097818461</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215">
         <f t="shared" ca="1" si="3"/>
-        <v>55224.578246802899</v>
+        <v>55309.110230702783</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216">
         <f t="shared" ca="1" si="3"/>
-        <v>88781.418124705029</v>
+        <v>78603.565108955809</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217">
         <f t="shared" ca="1" si="3"/>
-        <v>46003.78465644399</v>
+        <v>18837.272970604245</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218">
         <f t="shared" ca="1" si="3"/>
-        <v>82525.636527848721</v>
+        <v>69041.247371724981</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219">
         <f t="shared" ca="1" si="3"/>
-        <v>36859.557891242388</v>
+        <v>11851.399601397217</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220">
         <f t="shared" ca="1" si="3"/>
-        <v>96508.026273061318</v>
+        <v>18312.165825789572</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221">
         <f t="shared" ca="1" si="3"/>
-        <v>22970.52263386199</v>
+        <v>55503.724607265256</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222">
         <f t="shared" ca="1" si="3"/>
-        <v>3892.3330850986317</v>
+        <v>46419.60249128173</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223">
         <f t="shared" ca="1" si="3"/>
-        <v>32260.874952237027</v>
+        <v>53791.084517675481</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224">
         <f t="shared" ca="1" si="3"/>
-        <v>25197.90684541162</v>
+        <v>76787.422498239161</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225">
         <f t="shared" ca="1" si="3"/>
-        <v>77677.324049831383</v>
+        <v>92033.954445302239</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226">
         <f t="shared" ca="1" si="3"/>
-        <v>70790.50916116884</v>
+        <v>58515.389665960131</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227">
         <f t="shared" ca="1" si="3"/>
-        <v>51442.856384552382</v>
+        <v>35584.16825849696</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228">
         <f t="shared" ca="1" si="3"/>
-        <v>16247.115536193136</v>
+        <v>78200.785174695877</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229">
         <f t="shared" ca="1" si="3"/>
-        <v>30047.135158470552</v>
+        <v>87471.126090596517</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230">
         <f t="shared" ca="1" si="3"/>
-        <v>82151.898143501807</v>
+        <v>35728.988068188868</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231">
         <f t="shared" ca="1" si="3"/>
-        <v>67858.557472488013</v>
+        <v>41413.211378591652</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232">
         <f t="shared" ca="1" si="3"/>
-        <v>17757.638795555664</v>
+        <v>27097.428385603595</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233">
         <f t="shared" ca="1" si="3"/>
-        <v>84558.298382090652</v>
+        <v>54442.126599526076</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234">
         <f t="shared" ca="1" si="3"/>
-        <v>75572.999171182251</v>
+        <v>84075.291154467763</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235">
         <f t="shared" ca="1" si="3"/>
-        <v>2700.8823088953691</v>
+        <v>33448.885960508647</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236">
         <f t="shared" ca="1" si="3"/>
-        <v>5761.1449139674751</v>
+        <v>65702.064160220296</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237">
         <f t="shared" ca="1" si="3"/>
-        <v>81517.257199762666</v>
+        <v>54405.380802787608</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238">
         <f t="shared" ca="1" si="3"/>
-        <v>55768.610295430262</v>
+        <v>96321.972656819911</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239">
         <f t="shared" ca="1" si="3"/>
-        <v>61238.083510567121</v>
+        <v>64477.486160362459</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240">
         <f t="shared" ca="1" si="3"/>
-        <v>96980.226715197277</v>
+        <v>58873.827353960405</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241">
         <f t="shared" ca="1" si="3"/>
-        <v>7342.0264687767303</v>
+        <v>59363.812157249529</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242">
         <f t="shared" ca="1" si="3"/>
-        <v>35772.166174508915</v>
+        <v>73963.273065082627</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243">
         <f t="shared" ca="1" si="3"/>
-        <v>33395.668871329952</v>
+        <v>10078.857389139994</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244">
         <f t="shared" ca="1" si="3"/>
-        <v>14161.841410025278</v>
+        <v>82807.556000062221</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245">
         <f t="shared" ca="1" si="3"/>
-        <v>77871.219097470297</v>
+        <v>465.04584210301789</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246">
         <f t="shared" ca="1" si="3"/>
-        <v>83126.594702170827</v>
+        <v>60910.721585310726</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247">
         <f t="shared" ca="1" si="3"/>
-        <v>4645.9882179532897</v>
+        <v>3998.9972589245635</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248">
         <f t="shared" ca="1" si="3"/>
-        <v>63940.620832052839</v>
+        <v>53161.824777562775</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249">
         <f t="shared" ca="1" si="3"/>
-        <v>30474.700528272526</v>
+        <v>29376.264811522702</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250">
         <f t="shared" ca="1" si="3"/>
-        <v>6090.5161952104045</v>
+        <v>55083.38658417097</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251">
         <f t="shared" ca="1" si="3"/>
-        <v>93840.346676554822</v>
+        <v>38405.900334826591</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252">
         <f t="shared" ca="1" si="3"/>
-        <v>34670.464343428721</v>
+        <v>73478.395974108891</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253">
         <f t="shared" ca="1" si="3"/>
-        <v>90898.712975472154</v>
+        <v>99316.929867325292</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254">
         <f t="shared" ca="1" si="3"/>
-        <v>43858.063586972276</v>
+        <v>38348.157963976046</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255">
         <f t="shared" ca="1" si="3"/>
-        <v>26608.391158330825</v>
+        <v>14624.040600028442</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256">
         <f t="shared" ca="1" si="3"/>
-        <v>11525.947023385641</v>
+        <v>98280.464798336325</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257">
         <f t="shared" ca="1" si="3"/>
-        <v>61399.044939039151</v>
+        <v>41555.783845590391</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258">
         <f t="shared" ref="A258:A300" ca="1" si="4">RAND()*100000</f>
-        <v>82398.180209832339</v>
+        <v>93960.39172811665</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259">
         <f t="shared" ca="1" si="4"/>
-        <v>54773.059608040916</v>
+        <v>41439.670135745153</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260">
         <f t="shared" ca="1" si="4"/>
-        <v>34153.228865396588</v>
+        <v>85896.37170291254</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261">
         <f t="shared" ca="1" si="4"/>
-        <v>78239.835496558037</v>
+        <v>48878.102718517592</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262">
         <f t="shared" ca="1" si="4"/>
-        <v>72175.718617623177</v>
+        <v>82774.084183067316</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263">
         <f t="shared" ca="1" si="4"/>
-        <v>17295.40745994994</v>
+        <v>27658.091928585014</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264">
         <f t="shared" ca="1" si="4"/>
-        <v>72825.422947292638</v>
+        <v>47645.869029743946</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265">
         <f t="shared" ca="1" si="4"/>
-        <v>82255.314057179843</v>
+        <v>87608.407617581703</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266">
         <f t="shared" ca="1" si="4"/>
-        <v>47736.893705585346</v>
+        <v>3272.6282567145272</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267">
         <f t="shared" ca="1" si="4"/>
-        <v>72472.475966083701</v>
+        <v>19327.792978634428</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268">
         <f t="shared" ca="1" si="4"/>
-        <v>66745.667509155057</v>
+        <v>43449.27428146387</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269">
         <f t="shared" ca="1" si="4"/>
-        <v>65911.235112142036</v>
+        <v>43118.904124179193</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270">
         <f t="shared" ca="1" si="4"/>
-        <v>66087.485839363959</v>
+        <v>49738.052879837356</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271">
         <f t="shared" ca="1" si="4"/>
-        <v>7063.2266534864766</v>
+        <v>46938.976843845972</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272">
         <f t="shared" ca="1" si="4"/>
-        <v>99746.433352463355</v>
+        <v>51817.529564234341</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273">
         <f t="shared" ca="1" si="4"/>
-        <v>56919.221749890734</v>
+        <v>59241.125343561231</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274">
         <f t="shared" ca="1" si="4"/>
-        <v>40394.941099183881</v>
+        <v>67694.445976026138</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275">
         <f t="shared" ca="1" si="4"/>
-        <v>74706.318994079047</v>
+        <v>6458.3379634091334</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276">
         <f t="shared" ca="1" si="4"/>
-        <v>39853.216130302259</v>
+        <v>93382.845951338037</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277">
         <f t="shared" ca="1" si="4"/>
-        <v>13488.706869682876</v>
+        <v>57924.784014930163</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278">
         <f t="shared" ca="1" si="4"/>
-        <v>58448.749136200116</v>
+        <v>99898.434093078977</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279">
         <f t="shared" ca="1" si="4"/>
-        <v>24543.815693203862</v>
+        <v>13365.065441937906</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280">
         <f t="shared" ca="1" si="4"/>
-        <v>83638.413421729914</v>
+        <v>8737.1221529777158</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281">
         <f t="shared" ca="1" si="4"/>
-        <v>4073.7244698482168</v>
+        <v>69915.168766462593</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282">
         <f t="shared" ca="1" si="4"/>
-        <v>27822.395362111052</v>
+        <v>57674.2972747858</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283">
         <f t="shared" ca="1" si="4"/>
-        <v>79012.311325501665</v>
+        <v>9025.7569487288474</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284">
         <f t="shared" ca="1" si="4"/>
-        <v>57404.861768553375</v>
+        <v>13549.129062867949</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285">
         <f t="shared" ca="1" si="4"/>
-        <v>5675.5297798805395</v>
+        <v>98341.688771313711</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286">
         <f t="shared" ca="1" si="4"/>
-        <v>22729.960933276427</v>
+        <v>33136.166796343525</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287">
         <f t="shared" ca="1" si="4"/>
-        <v>82866.736177261278</v>
+        <v>56180.929678484026</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288">
         <f t="shared" ca="1" si="4"/>
-        <v>15051.385545403129</v>
+        <v>90186.318875095734</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289">
         <f t="shared" ca="1" si="4"/>
-        <v>12421.726238070585</v>
+        <v>52279.517106091502</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290">
         <f t="shared" ca="1" si="4"/>
-        <v>68579.0055509784</v>
+        <v>59348.339463492339</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291">
         <f t="shared" ca="1" si="4"/>
-        <v>42084.700717781954</v>
+        <v>156.89174032037511</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292">
         <f t="shared" ca="1" si="4"/>
-        <v>39060.453083498411</v>
+        <v>54776.516719444633</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293">
         <f t="shared" ca="1" si="4"/>
-        <v>4602.953207012617</v>
+        <v>1010.9120718179154</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294">
         <f t="shared" ca="1" si="4"/>
-        <v>19831.861716154897</v>
+        <v>54152.017992882909</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295">
         <f t="shared" ca="1" si="4"/>
-        <v>37949.363409906648</v>
+        <v>44259.778415917259</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296">
         <f t="shared" ca="1" si="4"/>
-        <v>47668.852325612534</v>
+        <v>23586.427946053478</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297">
         <f t="shared" ca="1" si="4"/>
-        <v>17317.842955806907</v>
+        <v>73806.288110769528</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298">
         <f t="shared" ca="1" si="4"/>
-        <v>98155.627250343037</v>
+        <v>11915.139271752905</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299">
         <f t="shared" ca="1" si="4"/>
-        <v>13838.979409774987</v>
+        <v>33923.119042630758</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300">
         <f t="shared" ca="1" si="4"/>
-        <v>66869.223324232371</v>
+        <v>539.45364274181622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update base de datos
</commit_message>
<xml_diff>
--- a/src/assets/data/BD_INVITADOS.xlsx
+++ b/src/assets/data/BD_INVITADOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Claudia Documentos\CYB\proyectos\angular\AppWedding\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{350F8882-EA00-4DA9-8BB5-AF500F2FEDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB157F33-1F95-48F2-8E7F-D702EC303941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="128">
   <si>
     <t>invitado</t>
   </si>
@@ -413,6 +413,18 @@
   </si>
   <si>
     <t>BC0000055</t>
+  </si>
+  <si>
+    <t>Wendy Kathleen Lozano</t>
+  </si>
+  <si>
+    <t>BC0000056</t>
+  </si>
+  <si>
+    <t>Jean Guevara Pozo</t>
+  </si>
+  <si>
+    <t>BC0000057</t>
   </si>
 </sst>
 </file>
@@ -801,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1345,7 +1357,7 @@
         <v>41</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="2"/>
@@ -2772,6 +2784,76 @@
         <v>36</v>
       </c>
       <c r="J56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" ref="C57" si="10">CONCATENATE(E57,F57)</f>
+        <v>BC000005642456</v>
+      </c>
+      <c r="D57">
+        <v>968238268</v>
+      </c>
+      <c r="E57" t="s">
+        <v>125</v>
+      </c>
+      <c r="F57">
+        <f>Hoja2!B57</f>
+        <v>42456</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" ref="H57" si="11">CONCATENATE(G57,C57)</f>
+        <v>https://bvasquez-code.github.io/AppWedding/?id=BC000005642456</v>
+      </c>
+      <c r="I57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" ref="C58" si="12">CONCATENATE(E58,F58)</f>
+        <v>BC00000577410</v>
+      </c>
+      <c r="D58">
+        <v>968238269</v>
+      </c>
+      <c r="E58" t="s">
+        <v>127</v>
+      </c>
+      <c r="F58">
+        <f>Hoja2!B58</f>
+        <v>7410</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" ref="H58" si="13">CONCATENATE(G58,C58)</f>
+        <v>https://bvasquez-code.github.io/AppWedding/?id=BC00000577410</v>
+      </c>
+      <c r="I58" t="s">
+        <v>36</v>
+      </c>
+      <c r="J58" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2784,9 +2866,11 @@
     <hyperlink ref="G54" r:id="rId3" xr:uid="{2E0D1352-D939-471C-AD35-0E844912A9E5}"/>
     <hyperlink ref="G55" r:id="rId4" xr:uid="{0D5BE78C-10A9-43FF-B267-27F08103036D}"/>
     <hyperlink ref="G56" r:id="rId5" xr:uid="{584BEC43-ACEA-4164-A957-EDA521A25576}"/>
+    <hyperlink ref="G57" r:id="rId6" xr:uid="{8657F787-11A6-4934-AF7C-53EE8CBF9C77}"/>
+    <hyperlink ref="G58" r:id="rId7" xr:uid="{1C08DE60-2F05-4EBF-9729-6BBCE42EEB8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -5519,1801 +5603,1801 @@
     <row r="1" spans="1:1">
       <c r="A1">
         <f ca="1">RAND()*100000</f>
-        <v>21115.554414910865</v>
+        <v>71741.23772595331</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
         <f t="shared" ref="A2:A65" ca="1" si="0">RAND()*100000</f>
-        <v>22514.582923385162</v>
+        <v>14881.501202227199</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>74399.269445892656</v>
+        <v>22493.425363614762</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>78515.276898167373</v>
+        <v>88475.376463408815</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>77391.563775532806</v>
+        <v>30622.409269179461</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>91443.753091155668</v>
+        <v>7177.8005388250294</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>25349.066452612478</v>
+        <v>88170.262171114548</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>17157.067216419553</v>
+        <v>29865.519174513756</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>77600.459418489569</v>
+        <v>81603.793702655268</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>73557.512981725115</v>
+        <v>83842.926907580608</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>6252.7004731963489</v>
+        <v>30864.85071119569</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>92722.024700761875</v>
+        <v>97911.155037846693</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>15258.75031105468</v>
+        <v>29017.541813797976</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>9230.8703068469604</v>
+        <v>72946.783644585361</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>96676.972342598048</v>
+        <v>17841.328897016272</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>22965.159643125076</v>
+        <v>31824.467352569209</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>10445.034623320049</v>
+        <v>23826.328790551288</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>99660.303590231182</v>
+        <v>25627.569790776171</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
         <f ca="1">RAND()*100000</f>
-        <v>53595.558207767201</v>
+        <v>90413.2626217871</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>44389.836071636848</v>
+        <v>59514.752357283221</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>12644.952415606669</v>
+        <v>55575.805426229264</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>39605.180047616392</v>
+        <v>31256.969013004964</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>98493.433831027694</v>
+        <v>46185.991265801182</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>70534.866109582043</v>
+        <v>83541.523549227466</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>74708.368481646874</v>
+        <v>74198.268468786264</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>84558.916440584391</v>
+        <v>25441.379337538448</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>5885.6180681898795</v>
+        <v>17290.914145047311</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>70047.750295533202</v>
+        <v>48781.593238792288</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>4488.6616306845099</v>
+        <v>81201.533402292582</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>11393.434203898878</v>
+        <v>221.17169210963405</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>64451.815744012696</v>
+        <v>10079.206485423609</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>79632.528825461646</v>
+        <v>6529.6598210338507</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>52528.662706146177</v>
+        <v>95107.466322624867</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>66781.314740797825</v>
+        <v>82002.647290730121</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>64801.43026364562</v>
+        <v>24412.952143580602</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>38320.337831034747</v>
+        <v>50541.080198149488</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>91777.984762481428</v>
+        <v>8567.9674284720895</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>5442.931448801547</v>
+        <v>28763.687129247828</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>21924.160142591354</v>
+        <v>6082.1702707816175</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>66594.144444345016</v>
+        <v>53373.947407076696</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>56461.968284601091</v>
+        <v>56048.677153633245</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>11994.62924679463</v>
+        <v>12704.562704801536</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>22999.172053284656</v>
+        <v>25720.259565103344</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>35091.576183708697</v>
+        <v>79230.226195417054</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>11892.220387242025</v>
+        <v>68212.124348627985</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>17954.016866272716</v>
+        <v>28904.057702774931</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>19385.066650194927</v>
+        <v>11597.346093094919</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>3340.3089056936788</v>
+        <v>25750.874456660746</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>24928.739518060862</v>
+        <v>55217.702755124177</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>93907.649428615274</v>
+        <v>57820.522381657756</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>56253.450074198474</v>
+        <v>76463.048144883433</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>47328.779004261014</v>
+        <v>39074.354360900645</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>14029.928643825751</v>
+        <v>90923.812472382619</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>75739.34370457867</v>
+        <v>49302.306467944967</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>72862.841575161758</v>
+        <v>1508.1933954906201</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>70683.42335323905</v>
+        <v>10347.176904081589</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>36913.739184451057</v>
+        <v>73210.953725977204</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>27966.831106030819</v>
+        <v>61789.994215491592</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>6932.3087299021372</v>
+        <v>72101.008866385499</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>62915.906651122546</v>
+        <v>25076.004344804871</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>88588.666697631328</v>
+        <v>38738.708291627569</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>37345.489219038798</v>
+        <v>7913.8927410355773</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>31593.624302280175</v>
+        <v>48543.102068420005</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>18973.703618220228</v>
+        <v>66907.983966386993</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
         <f t="shared" ca="1" si="0"/>
-        <v>60106.811043329966</v>
+        <v>7094.567206684399</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
         <f t="shared" ref="A66:A129" ca="1" si="1">RAND()*100000</f>
-        <v>40265.690163120162</v>
+        <v>36402.770340185096</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
         <f t="shared" ca="1" si="1"/>
-        <v>40947.444534098722</v>
+        <v>11464.981793992001</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
         <f t="shared" ca="1" si="1"/>
-        <v>41190.179926859746</v>
+        <v>1364.8042568687902</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
         <f t="shared" ca="1" si="1"/>
-        <v>48866.437083633173</v>
+        <v>48272.19718603044</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
         <f t="shared" ca="1" si="1"/>
-        <v>39383.022187626651</v>
+        <v>54332.427733943965</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
         <f t="shared" ca="1" si="1"/>
-        <v>48446.848762560156</v>
+        <v>32376.224921814188</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
         <f t="shared" ca="1" si="1"/>
-        <v>71775.850167201846</v>
+        <v>92320.357745146015</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
         <f t="shared" ca="1" si="1"/>
-        <v>43302.891363860566</v>
+        <v>28313.405524234138</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
         <f t="shared" ca="1" si="1"/>
-        <v>26566.547504356164</v>
+        <v>91897.274077552531</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
         <f t="shared" ca="1" si="1"/>
-        <v>51045.102827713439</v>
+        <v>80470.009701306903</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
         <f t="shared" ca="1" si="1"/>
-        <v>21568.207197213109</v>
+        <v>76130.651851727525</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
         <f t="shared" ca="1" si="1"/>
-        <v>6973.6048820452033</v>
+        <v>86303.98488801028</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
         <f t="shared" ca="1" si="1"/>
-        <v>42740.284961475569</v>
+        <v>89455.483141838034</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
         <f t="shared" ca="1" si="1"/>
-        <v>23924.513871697971</v>
+        <v>11944.709663842301</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
         <f t="shared" ca="1" si="1"/>
-        <v>54124.261162798874</v>
+        <v>23796.815462957689</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
         <f t="shared" ca="1" si="1"/>
-        <v>77389.718901411266</v>
+        <v>58089.064028547058</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
         <f t="shared" ca="1" si="1"/>
-        <v>48776.346552849871</v>
+        <v>96972.467669758189</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83">
         <f t="shared" ca="1" si="1"/>
-        <v>78838.764909384307</v>
+        <v>17959.543370578245</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84">
         <f t="shared" ca="1" si="1"/>
-        <v>73612.033610421044</v>
+        <v>9937.6591219923375</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
         <f t="shared" ca="1" si="1"/>
-        <v>40799.803557942469</v>
+        <v>30061.213251090379</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86">
         <f t="shared" ca="1" si="1"/>
-        <v>12947.143873029143</v>
+        <v>72993.13124339249</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87">
         <f t="shared" ca="1" si="1"/>
-        <v>68939.172118342423</v>
+        <v>94325.062674881949</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88">
         <f t="shared" ca="1" si="1"/>
-        <v>42306.877321950786</v>
+        <v>67864.9860918841</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89">
         <f t="shared" ca="1" si="1"/>
-        <v>36138.928585665395</v>
+        <v>79178.810710767648</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
         <f t="shared" ca="1" si="1"/>
-        <v>75275.757561693608</v>
+        <v>93928.340311844426</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
         <f t="shared" ca="1" si="1"/>
-        <v>50612.780503090406</v>
+        <v>23236.02594907751</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
         <f t="shared" ca="1" si="1"/>
-        <v>71803.407877149075</v>
+        <v>79487.637954320337</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
         <f t="shared" ca="1" si="1"/>
-        <v>93073.134735240601</v>
+        <v>41549.03067150533</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
         <f t="shared" ca="1" si="1"/>
-        <v>49560.884366767597</v>
+        <v>19562.541252177267</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
         <f t="shared" ca="1" si="1"/>
-        <v>98763.084339496869</v>
+        <v>60627.933306892337</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
         <f t="shared" ca="1" si="1"/>
-        <v>16899.482326905534</v>
+        <v>1473.8680761244627</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97">
         <f t="shared" ca="1" si="1"/>
-        <v>93942.596257140976</v>
+        <v>21046.637394101908</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
         <f t="shared" ca="1" si="1"/>
-        <v>43791.404103808571</v>
+        <v>7099.4060698422845</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
         <f t="shared" ca="1" si="1"/>
-        <v>94759.74231450395</v>
+        <v>89250.443852426717</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
         <f t="shared" ca="1" si="1"/>
-        <v>55194.287625679128</v>
+        <v>97925.36958653995</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
         <f t="shared" ca="1" si="1"/>
-        <v>71316.372089892044</v>
+        <v>98392.918412157975</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
         <f t="shared" ca="1" si="1"/>
-        <v>31210.016088051219</v>
+        <v>67588.303179665731</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
         <f t="shared" ca="1" si="1"/>
-        <v>9965.1800505371812</v>
+        <v>88939.658245579762</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104">
         <f t="shared" ca="1" si="1"/>
-        <v>57394.873482671203</v>
+        <v>99013.758367054979</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
         <f t="shared" ca="1" si="1"/>
-        <v>12826.899191746854</v>
+        <v>79089.140189515281</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106">
         <f t="shared" ca="1" si="1"/>
-        <v>95949.028178942826</v>
+        <v>94730.335786198819</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107">
         <f t="shared" ca="1" si="1"/>
-        <v>69077.056427514981</v>
+        <v>92276.332580158953</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
         <f t="shared" ca="1" si="1"/>
-        <v>98988.558232464682</v>
+        <v>77935.364278613662</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
         <f t="shared" ca="1" si="1"/>
-        <v>92551.181388824683</v>
+        <v>37343.089284809917</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
         <f t="shared" ca="1" si="1"/>
-        <v>69438.762436300036</v>
+        <v>26458.622691147993</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
         <f t="shared" ca="1" si="1"/>
-        <v>36626.115158463224</v>
+        <v>53582.893887236634</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
         <f t="shared" ca="1" si="1"/>
-        <v>3764.1165506240413</v>
+        <v>16042.370927888205</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113">
         <f t="shared" ca="1" si="1"/>
-        <v>21504.030400408079</v>
+        <v>92593.664665314252</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
         <f t="shared" ca="1" si="1"/>
-        <v>24360.920783357185</v>
+        <v>8257.5064156369608</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115">
         <f t="shared" ca="1" si="1"/>
-        <v>56722.550120540152</v>
+        <v>17053.595929974163</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116">
         <f t="shared" ca="1" si="1"/>
-        <v>27470.972431465023</v>
+        <v>7022.7146415789866</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117">
         <f t="shared" ca="1" si="1"/>
-        <v>18947.338227888198</v>
+        <v>73470.751839067962</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118">
         <f t="shared" ca="1" si="1"/>
-        <v>93862.672759088688</v>
+        <v>34792.236088046055</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119">
         <f t="shared" ca="1" si="1"/>
-        <v>16822.837208555509</v>
+        <v>99031.645398565684</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120">
         <f t="shared" ca="1" si="1"/>
-        <v>49825.385737922436</v>
+        <v>9810.712643214647</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
         <f t="shared" ca="1" si="1"/>
-        <v>25524.241302244012</v>
+        <v>8926.9406709021496</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122">
         <f t="shared" ca="1" si="1"/>
-        <v>30068.563522871184</v>
+        <v>12178.073787912303</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123">
         <f t="shared" ca="1" si="1"/>
-        <v>63661.861467692892</v>
+        <v>43751.577057268441</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124">
         <f t="shared" ca="1" si="1"/>
-        <v>8174.9510335789146</v>
+        <v>31736.823334612251</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125">
         <f t="shared" ca="1" si="1"/>
-        <v>94503.818621440223</v>
+        <v>52035.634750333746</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126">
         <f t="shared" ca="1" si="1"/>
-        <v>19758.707204091632</v>
+        <v>91903.224387564958</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127">
         <f t="shared" ca="1" si="1"/>
-        <v>85905.986615174406</v>
+        <v>56580.044448828026</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128">
         <f t="shared" ca="1" si="1"/>
-        <v>43717.06682598636</v>
+        <v>9195.2783273175792</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129">
         <f t="shared" ca="1" si="1"/>
-        <v>26282.357914702847</v>
+        <v>27553.425761152517</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130">
         <f t="shared" ref="A130:A193" ca="1" si="2">RAND()*100000</f>
-        <v>12025.030302085916</v>
+        <v>42774.669358258754</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131">
         <f t="shared" ca="1" si="2"/>
-        <v>57729.921488016524</v>
+        <v>37350.330310942394</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132">
         <f t="shared" ca="1" si="2"/>
-        <v>8206.3494494194929</v>
+        <v>39657.918893346177</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133">
         <f t="shared" ca="1" si="2"/>
-        <v>91244.4615560495</v>
+        <v>44490.440814203248</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134">
         <f t="shared" ca="1" si="2"/>
-        <v>12827.228949427748</v>
+        <v>86580.663352869713</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135">
         <f t="shared" ca="1" si="2"/>
-        <v>36488.648700891114</v>
+        <v>58894.391790914735</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136">
         <f t="shared" ca="1" si="2"/>
-        <v>70080.549450978549</v>
+        <v>84353.185785053443</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137">
         <f t="shared" ca="1" si="2"/>
-        <v>59497.762766156018</v>
+        <v>81536.999545829065</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138">
         <f t="shared" ca="1" si="2"/>
-        <v>38.362545679437865</v>
+        <v>28010.8183171649</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139">
         <f t="shared" ca="1" si="2"/>
-        <v>80872.065655258979</v>
+        <v>16429.453150534468</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140">
         <f t="shared" ca="1" si="2"/>
-        <v>64259.334099800501</v>
+        <v>65424.395049231374</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141">
         <f t="shared" ca="1" si="2"/>
-        <v>47841.784201190276</v>
+        <v>65571.832624254166</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
         <f t="shared" ca="1" si="2"/>
-        <v>67712.367898062061</v>
+        <v>9702.9795237185681</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
         <f t="shared" ca="1" si="2"/>
-        <v>6556.9139230675974</v>
+        <v>85659.749829078108</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144">
         <f t="shared" ca="1" si="2"/>
-        <v>28137.038915400415</v>
+        <v>86805.088708865878</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145">
         <f t="shared" ca="1" si="2"/>
-        <v>30700.925222714624</v>
+        <v>8700.3765372241196</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146">
         <f t="shared" ca="1" si="2"/>
-        <v>56659.787003566045</v>
+        <v>23218.502232074588</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147">
         <f t="shared" ca="1" si="2"/>
-        <v>49020.810065647434</v>
+        <v>34718.247366604061</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148">
         <f t="shared" ca="1" si="2"/>
-        <v>20823.903722709423</v>
+        <v>52293.637021352777</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
         <f t="shared" ca="1" si="2"/>
-        <v>76013.261848848415</v>
+        <v>75098.781673347708</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150">
         <f t="shared" ca="1" si="2"/>
-        <v>45459.591833270308</v>
+        <v>24075.71231565937</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151">
         <f t="shared" ca="1" si="2"/>
-        <v>13672.882546139497</v>
+        <v>75314.914438790933</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
         <f t="shared" ca="1" si="2"/>
-        <v>77647.218217923539</v>
+        <v>22034.294274683354</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153">
         <f t="shared" ca="1" si="2"/>
-        <v>26149.965493819825</v>
+        <v>51644.119036161872</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
         <f t="shared" ca="1" si="2"/>
-        <v>52489.53666263607</v>
+        <v>61056.769781504161</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155">
         <f t="shared" ca="1" si="2"/>
-        <v>66505.237700434212</v>
+        <v>88652.351030308811</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156">
         <f t="shared" ca="1" si="2"/>
-        <v>24707.32499776176</v>
+        <v>54703.261695054418</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157">
         <f t="shared" ca="1" si="2"/>
-        <v>45648.647599880875</v>
+        <v>9221.8906858324008</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158">
         <f t="shared" ca="1" si="2"/>
-        <v>33295.20661185935</v>
+        <v>74126.81278911003</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159">
         <f t="shared" ca="1" si="2"/>
-        <v>89663.322760120893</v>
+        <v>16844.050538990297</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160">
         <f t="shared" ca="1" si="2"/>
-        <v>55973.023117157849</v>
+        <v>35746.528821177337</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161">
         <f t="shared" ca="1" si="2"/>
-        <v>98746.968529351652</v>
+        <v>58988.158393219615</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162">
         <f t="shared" ca="1" si="2"/>
-        <v>35837.800660641027</v>
+        <v>67198.815129007198</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163">
         <f t="shared" ca="1" si="2"/>
-        <v>27252.977499757159</v>
+        <v>71582.005494194862</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164">
         <f t="shared" ca="1" si="2"/>
-        <v>68682.860087967289</v>
+        <v>39897.844719385153</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165">
         <f t="shared" ca="1" si="2"/>
-        <v>61267.308155056446</v>
+        <v>51604.921586854471</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166">
         <f t="shared" ca="1" si="2"/>
-        <v>99581.618628022887</v>
+        <v>79816.766472566029</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167">
         <f t="shared" ca="1" si="2"/>
-        <v>67797.71975502788</v>
+        <v>97934.343287331372</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168">
         <f t="shared" ca="1" si="2"/>
-        <v>81853.070513824307</v>
+        <v>66757.501478080085</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169">
         <f t="shared" ca="1" si="2"/>
-        <v>6575.5211481844381</v>
+        <v>10493.258161710339</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170">
         <f t="shared" ca="1" si="2"/>
-        <v>24446.513961864512</v>
+        <v>67342.062854148055</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171">
         <f t="shared" ca="1" si="2"/>
-        <v>70242.362030858276</v>
+        <v>82848.839176489535</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
         <f t="shared" ca="1" si="2"/>
-        <v>31282.225125149111</v>
+        <v>50793.992428620615</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
         <f t="shared" ca="1" si="2"/>
-        <v>19513.791729790275</v>
+        <v>81519.593190017928</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174">
         <f t="shared" ca="1" si="2"/>
-        <v>77738.413170795713</v>
+        <v>63972.376049016711</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
         <f t="shared" ca="1" si="2"/>
-        <v>8967.778866671817</v>
+        <v>88616.390535707294</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
         <f t="shared" ca="1" si="2"/>
-        <v>31545.841661317099</v>
+        <v>67315.28519767434</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177">
         <f t="shared" ca="1" si="2"/>
-        <v>60088.977904430853</v>
+        <v>4103.5094886271218</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178">
         <f t="shared" ca="1" si="2"/>
-        <v>52259.642047573449</v>
+        <v>2380.0650527048829</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179">
         <f t="shared" ca="1" si="2"/>
-        <v>18564.865820639709</v>
+        <v>38121.924066461201</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180">
         <f t="shared" ca="1" si="2"/>
-        <v>64664.074216301357</v>
+        <v>43176.9996722098</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181">
         <f t="shared" ca="1" si="2"/>
-        <v>34681.345164692953</v>
+        <v>25769.176674264305</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182">
         <f t="shared" ca="1" si="2"/>
-        <v>58648.71663350294</v>
+        <v>7335.6746698031602</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183">
         <f t="shared" ca="1" si="2"/>
-        <v>28867.145751783995</v>
+        <v>45499.529696825157</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184">
         <f t="shared" ca="1" si="2"/>
-        <v>78325.788879707543</v>
+        <v>15653.771709611674</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185">
         <f t="shared" ca="1" si="2"/>
-        <v>96743.128553580391</v>
+        <v>60954.58066010895</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186">
         <f t="shared" ca="1" si="2"/>
-        <v>86316.075744256043</v>
+        <v>734.15607011427801</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
         <f t="shared" ca="1" si="2"/>
-        <v>33330.870158429861</v>
+        <v>63114.266392199279</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188">
         <f t="shared" ca="1" si="2"/>
-        <v>46137.239891547419</v>
+        <v>48527.539329938285</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189">
         <f t="shared" ca="1" si="2"/>
-        <v>31743.51969756186</v>
+        <v>95386.729875438119</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190">
         <f t="shared" ca="1" si="2"/>
-        <v>82746.196997300198</v>
+        <v>38084.014728703318</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191">
         <f t="shared" ca="1" si="2"/>
-        <v>78495.995754448886</v>
+        <v>59589.34904174471</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192">
         <f t="shared" ca="1" si="2"/>
-        <v>73005.340268338681</v>
+        <v>98546.228476268065</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
         <f t="shared" ca="1" si="2"/>
-        <v>75345.542104970751</v>
+        <v>20935.975487743275</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194">
         <f t="shared" ref="A194:A257" ca="1" si="3">RAND()*100000</f>
-        <v>39249.874469062452</v>
+        <v>50017.140066965825</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195">
         <f t="shared" ca="1" si="3"/>
-        <v>89966.912325679819</v>
+        <v>97551.708173145758</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196">
         <f t="shared" ca="1" si="3"/>
-        <v>3376.5762295924319</v>
+        <v>11958.308541806351</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197">
         <f t="shared" ca="1" si="3"/>
-        <v>73144.451976245749</v>
+        <v>56244.764110175136</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198">
         <f t="shared" ca="1" si="3"/>
-        <v>4958.3704817021789</v>
+        <v>19700.969281234004</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199">
         <f t="shared" ca="1" si="3"/>
-        <v>85806.608454258778</v>
+        <v>5025.6044620949906</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200">
         <f t="shared" ca="1" si="3"/>
-        <v>17680.358421097786</v>
+        <v>11086.722210153932</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
         <f t="shared" ca="1" si="3"/>
-        <v>40831.659363039988</v>
+        <v>66047.273102292253</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
         <f t="shared" ca="1" si="3"/>
-        <v>14775.912696976857</v>
+        <v>3620.0996657054343</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
         <f t="shared" ca="1" si="3"/>
-        <v>34149.134742870025</v>
+        <v>1923.3403266088023</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204">
         <f t="shared" ca="1" si="3"/>
-        <v>84184.044697565332</v>
+        <v>63488.297765530835</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205">
         <f t="shared" ca="1" si="3"/>
-        <v>93661.828777944756</v>
+        <v>44137.852710773914</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
         <f t="shared" ca="1" si="3"/>
-        <v>89388.610572548816</v>
+        <v>45474.744382868339</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
         <f t="shared" ca="1" si="3"/>
-        <v>78354.484880809978</v>
+        <v>63745.240123092051</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
         <f t="shared" ca="1" si="3"/>
-        <v>99653.992828128568</v>
+        <v>68350.714631734663</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
         <f t="shared" ca="1" si="3"/>
-        <v>2257.1082280840483</v>
+        <v>67650.780998644463</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210">
         <f t="shared" ca="1" si="3"/>
-        <v>15147.394006294302</v>
+        <v>1959.7963561381105</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211">
         <f t="shared" ca="1" si="3"/>
-        <v>65924.067258491079</v>
+        <v>97265.728780913836</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212">
         <f t="shared" ca="1" si="3"/>
-        <v>5859.3557944751519</v>
+        <v>2439.9266523525198</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213">
         <f t="shared" ca="1" si="3"/>
-        <v>261.40736520290363</v>
+        <v>63793.865386589423</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214">
         <f t="shared" ca="1" si="3"/>
-        <v>67709.129112104783</v>
+        <v>68539.300007279162</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215">
         <f t="shared" ca="1" si="3"/>
-        <v>97298.112105353997</v>
+        <v>17281.419500794316</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
         <f t="shared" ca="1" si="3"/>
-        <v>25358.972303868697</v>
+        <v>65763.177320356655</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217">
         <f t="shared" ca="1" si="3"/>
-        <v>61207.323603188372</v>
+        <v>35946.066108614417</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218">
         <f t="shared" ca="1" si="3"/>
-        <v>57304.075181652617</v>
+        <v>47101.899565318992</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219">
         <f t="shared" ca="1" si="3"/>
-        <v>3671.8766166937035</v>
+        <v>29096.763755637257</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220">
         <f t="shared" ca="1" si="3"/>
-        <v>30239.493376497627</v>
+        <v>36241.662909902792</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221">
         <f t="shared" ca="1" si="3"/>
-        <v>41571.929558432697</v>
+        <v>34732.700923461038</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
         <f t="shared" ca="1" si="3"/>
-        <v>3490.998577910831</v>
+        <v>54674.107965328534</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
         <f t="shared" ca="1" si="3"/>
-        <v>89691.996283505956</v>
+        <v>51249.5151210728</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224">
         <f t="shared" ca="1" si="3"/>
-        <v>24611.702303119397</v>
+        <v>90102.874100783796</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225">
         <f t="shared" ca="1" si="3"/>
-        <v>83615.863481158041</v>
+        <v>54830.525966583766</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226">
         <f t="shared" ca="1" si="3"/>
-        <v>13481.146792684118</v>
+        <v>62986.194332108593</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227">
         <f t="shared" ca="1" si="3"/>
-        <v>80875.22622377993</v>
+        <v>7767.928247709011</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228">
         <f t="shared" ca="1" si="3"/>
-        <v>92559.198950512888</v>
+        <v>37509.123884046247</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229">
         <f t="shared" ca="1" si="3"/>
-        <v>96571.902201903838</v>
+        <v>61657.52815558212</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230">
         <f t="shared" ca="1" si="3"/>
-        <v>38709.182314232028</v>
+        <v>68243.89222954365</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
         <f t="shared" ca="1" si="3"/>
-        <v>97101.106151352462</v>
+        <v>13434.56032730319</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232">
         <f t="shared" ca="1" si="3"/>
-        <v>58337.658147045993</v>
+        <v>8274.5465079101068</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233">
         <f t="shared" ca="1" si="3"/>
-        <v>35720.65927485811</v>
+        <v>3358.8272131814369</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234">
         <f t="shared" ca="1" si="3"/>
-        <v>8121.7005276163263</v>
+        <v>76978.654909308942</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235">
         <f t="shared" ca="1" si="3"/>
-        <v>33571.41069830428</v>
+        <v>62433.9505527578</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
         <f t="shared" ca="1" si="3"/>
-        <v>84340.445201169321</v>
+        <v>98725.077046591716</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
         <f t="shared" ca="1" si="3"/>
-        <v>75940.440352331934</v>
+        <v>46675.876111154837</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238">
         <f t="shared" ca="1" si="3"/>
-        <v>10118.930734242271</v>
+        <v>11266.3219088735</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239">
         <f t="shared" ca="1" si="3"/>
-        <v>34561.31456512458</v>
+        <v>41735.914524011787</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240">
         <f t="shared" ca="1" si="3"/>
-        <v>36212.473735746222</v>
+        <v>18715.043281882859</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241">
         <f t="shared" ca="1" si="3"/>
-        <v>53559.039892553592</v>
+        <v>25429.046907868757</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242">
         <f t="shared" ca="1" si="3"/>
-        <v>44263.038814464853</v>
+        <v>63765.074879700936</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243">
         <f t="shared" ca="1" si="3"/>
-        <v>54263.205090146672</v>
+        <v>57353.532653767594</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244">
         <f t="shared" ca="1" si="3"/>
-        <v>14205.495022503479</v>
+        <v>757.81335414603075</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245">
         <f t="shared" ca="1" si="3"/>
-        <v>43057.400732355774</v>
+        <v>41400.061583075942</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246">
         <f t="shared" ca="1" si="3"/>
-        <v>79155.817510515088</v>
+        <v>44485.100330726214</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247">
         <f t="shared" ca="1" si="3"/>
-        <v>60683.855738145619</v>
+        <v>70920.300565776299</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248">
         <f t="shared" ca="1" si="3"/>
-        <v>36898.696448510549</v>
+        <v>21672.71986381102</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249">
         <f t="shared" ca="1" si="3"/>
-        <v>36901.81698841574</v>
+        <v>10197.606303068575</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250">
         <f t="shared" ca="1" si="3"/>
-        <v>51571.446944990574</v>
+        <v>82650.971805824389</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
         <f t="shared" ca="1" si="3"/>
-        <v>35289.204041780111</v>
+        <v>83529.518048952901</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252">
         <f t="shared" ca="1" si="3"/>
-        <v>12991.775588648257</v>
+        <v>15045.110640456838</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253">
         <f t="shared" ca="1" si="3"/>
-        <v>89123.5328193819</v>
+        <v>47950.846625333819</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254">
         <f t="shared" ca="1" si="3"/>
-        <v>16547.32211931924</v>
+        <v>46076.368057254316</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
         <f t="shared" ca="1" si="3"/>
-        <v>41069.03801878322</v>
+        <v>53381.160999906475</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
         <f t="shared" ca="1" si="3"/>
-        <v>8555.4914115092979</v>
+        <v>69622.55761738462</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257">
         <f t="shared" ca="1" si="3"/>
-        <v>84462.771529981866</v>
+        <v>18784.154233165762</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258">
         <f t="shared" ref="A258:A300" ca="1" si="4">RAND()*100000</f>
-        <v>9974.4136271220814</v>
+        <v>96741.995118532286</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259">
         <f t="shared" ca="1" si="4"/>
-        <v>7217.9511617173948</v>
+        <v>98535.675509457593</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260">
         <f t="shared" ca="1" si="4"/>
-        <v>53671.158401411813</v>
+        <v>48682.222690884904</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
         <f t="shared" ca="1" si="4"/>
-        <v>65456.55877743286</v>
+        <v>40297.712012329823</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262">
         <f t="shared" ca="1" si="4"/>
-        <v>44928.566117604452</v>
+        <v>86017.099115268429</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263">
         <f t="shared" ca="1" si="4"/>
-        <v>56355.959384536705</v>
+        <v>44606.020570639863</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264">
         <f t="shared" ca="1" si="4"/>
-        <v>81170.623693118512</v>
+        <v>97467.905086392333</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265">
         <f t="shared" ca="1" si="4"/>
-        <v>66431.697029422619</v>
+        <v>13227.916677128747</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
         <f t="shared" ca="1" si="4"/>
-        <v>83004.538233523519</v>
+        <v>83038.236862080055</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
         <f t="shared" ca="1" si="4"/>
-        <v>83639.905454769803</v>
+        <v>49976.19947934767</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268">
         <f t="shared" ca="1" si="4"/>
-        <v>52939.87955149584</v>
+        <v>19684.966798104986</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269">
         <f t="shared" ca="1" si="4"/>
-        <v>54927.661473924883</v>
+        <v>8661.905390399028</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270">
         <f t="shared" ca="1" si="4"/>
-        <v>11591.425930573207</v>
+        <v>35701.18017063498</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271">
         <f t="shared" ca="1" si="4"/>
-        <v>85415.617430155646</v>
+        <v>47472.987404747837</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272">
         <f t="shared" ca="1" si="4"/>
-        <v>95314.655924899955</v>
+        <v>32255.751295888713</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273">
         <f t="shared" ca="1" si="4"/>
-        <v>91799.408972512465</v>
+        <v>97658.854143488497</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274">
         <f t="shared" ca="1" si="4"/>
-        <v>75457.036470974286</v>
+        <v>89875.736951181199</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275">
         <f t="shared" ca="1" si="4"/>
-        <v>17345.705634154398</v>
+        <v>59122.035543339283</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276">
         <f t="shared" ca="1" si="4"/>
-        <v>47078.808871971552</v>
+        <v>13825.13217620025</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277">
         <f t="shared" ca="1" si="4"/>
-        <v>60345.942748475303</v>
+        <v>21897.126454775851</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278">
         <f t="shared" ca="1" si="4"/>
-        <v>44896.954984834825</v>
+        <v>33162.604894269709</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279">
         <f t="shared" ca="1" si="4"/>
-        <v>8529.6541573298127</v>
+        <v>97968.416531413357</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
         <f t="shared" ca="1" si="4"/>
-        <v>33718.995051538899</v>
+        <v>61127.539216885249</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281">
         <f t="shared" ca="1" si="4"/>
-        <v>6762.6261257017759</v>
+        <v>65517.445162430267</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282">
         <f t="shared" ca="1" si="4"/>
-        <v>22162.089235778159</v>
+        <v>76115.82526581861</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283">
         <f t="shared" ca="1" si="4"/>
-        <v>99128.253687683071</v>
+        <v>89362.909544647904</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284">
         <f t="shared" ca="1" si="4"/>
-        <v>29345.899064927482</v>
+        <v>58334.904438976584</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285">
         <f t="shared" ca="1" si="4"/>
-        <v>83233.243475209005</v>
+        <v>69503.923333146638</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286">
         <f t="shared" ca="1" si="4"/>
-        <v>4266.6521870284414</v>
+        <v>31928.559314384041</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287">
         <f t="shared" ca="1" si="4"/>
-        <v>95335.674661009311</v>
+        <v>20316.89672576814</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288">
         <f t="shared" ca="1" si="4"/>
-        <v>46533.744244364985</v>
+        <v>36266.002662147534</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289">
         <f t="shared" ca="1" si="4"/>
-        <v>34018.323470126103</v>
+        <v>4723.8926591864129</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290">
         <f t="shared" ca="1" si="4"/>
-        <v>48289.477673358393</v>
+        <v>15495.029756743139</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291">
         <f t="shared" ca="1" si="4"/>
-        <v>40721.700952672159</v>
+        <v>35423.16542957705</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292">
         <f t="shared" ca="1" si="4"/>
-        <v>80438.176705415448</v>
+        <v>4878.4739908829924</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293">
         <f t="shared" ca="1" si="4"/>
-        <v>19695.361843806026</v>
+        <v>52867.894279928529</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294">
         <f t="shared" ca="1" si="4"/>
-        <v>8930.9467732711764</v>
+        <v>9349.2344994448704</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295">
         <f t="shared" ca="1" si="4"/>
-        <v>5194.3167075609645</v>
+        <v>38338.300450137707</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296">
         <f t="shared" ca="1" si="4"/>
-        <v>20265.805054445194</v>
+        <v>49531.190099136256</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297">
         <f t="shared" ca="1" si="4"/>
-        <v>93190.890775508611</v>
+        <v>26354.853082844766</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298">
         <f t="shared" ca="1" si="4"/>
-        <v>63846.954966670768</v>
+        <v>99547.932201216958</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299">
         <f t="shared" ca="1" si="4"/>
-        <v>91797.546231310916</v>
+        <v>96166.442220876532</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300">
         <f t="shared" ca="1" si="4"/>
-        <v>29201.46733428257</v>
+        <v>9261.518775145827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Base de datos actu
</commit_message>
<xml_diff>
--- a/src/assets/data/BD_INVITADOS.xlsx
+++ b/src/assets/data/BD_INVITADOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Claudia Documentos\CYB\proyectos\angular\AppWedding\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78576262-4A9E-4FCC-A155-DA599D649A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{730EFA14-9EAB-45DB-95A9-A0A1D98A14F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
     <t>BC0000037</t>
   </si>
   <si>
-    <t>Tía Rosa Irigorin</t>
+    <t>Madrina Rosa Irigoyen</t>
   </si>
   <si>
     <t>BC0000038</t>
@@ -827,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5687,1801 +5687,1801 @@
     <row r="1" spans="1:1">
       <c r="A1">
         <f ca="1">RAND()*100000</f>
-        <v>51906.488880815792</v>
+        <v>85067.404826532613</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
         <f t="shared" ref="A2:A65" ca="1" si="0">RAND()*100000</f>
-        <v>14600.546463545994</v>
+        <v>14678.606395003402</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>85601.682001853405</v>
+        <v>64134.512733769843</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>81547.317543451616</v>
+        <v>5816.9362648954784</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>18662.091980099794</v>
+        <v>71737.599512563742</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>15018.038477162465</v>
+        <v>33370.338328514168</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>84533.364704640699</v>
+        <v>90408.106400002696</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>75990.355002432276</v>
+        <v>90384.479038732738</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>10453.711071063155</v>
+        <v>42416.342413601778</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>4881.1221061678234</v>
+        <v>48150.95543227328</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>22576.827761837514</v>
+        <v>11461.023066338616</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>75682.42015781613</v>
+        <v>76813.102073948045</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>62098.142415279566</v>
+        <v>49138.635167716908</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>79126.599188031134</v>
+        <v>85012.16050646911</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>13134.276190075245</v>
+        <v>57366.020797394282</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>81988.107826880499</v>
+        <v>88428.02894183404</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>82693.740636398928</v>
+        <v>21734.95560118397</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>29736.80398973927</v>
+        <v>82175.876938671412</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
         <f ca="1">RAND()*100000</f>
-        <v>45648.401096770816</v>
+        <v>69005.413474072484</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>30831.737688289541</v>
+        <v>98127.185099524344</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>88098.342325780992</v>
+        <v>60207.171370550837</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>79069.749529753288</v>
+        <v>43929.708741002469</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>80415.62229043158</v>
+        <v>2375.5660559233947</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>23443.601535799975</v>
+        <v>97256.886328543376</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>34161.60152862384</v>
+        <v>10040.510278040059</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>13322.92574456122</v>
+        <v>48433.180896317339</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>87898.875419854216</v>
+        <v>797.51444921930533</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>91280.781818103351</v>
+        <v>59186.047358832097</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>52378.888637196542</v>
+        <v>18994.90681398892</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>30512.277796444199</v>
+        <v>84734.412437589301</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>27046.913384039784</v>
+        <v>76899.370714312448</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>34298.877764996039</v>
+        <v>33856.007867930806</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>18151.241583319756</v>
+        <v>93226.409729905266</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>51363.153113016022</v>
+        <v>73141.228919935224</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>6326.282902540881</v>
+        <v>33734.406240586897</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>33139.826614777521</v>
+        <v>13320.295398719072</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>22531.318743302621</v>
+        <v>55276.884274228709</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>21705.297270654479</v>
+        <v>1448.2581832727992</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>28082.613305280389</v>
+        <v>91358.720380199738</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>94558.726988376293</v>
+        <v>85739.575159019354</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>31384.362862058424</v>
+        <v>52490.329751902573</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>8814.6233066906279</v>
+        <v>43879.463030116764</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>46812.544619126325</v>
+        <v>92699.308312428693</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>84691.554864889258</v>
+        <v>9514.7688656819446</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>92177.690288193859</v>
+        <v>18601.835913852261</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>75089.217114597457</v>
+        <v>4362.6096085089048</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>89049.892551011159</v>
+        <v>74186.618233141286</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>92577.1044545638</v>
+        <v>44641.578558258712</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>46115.969388893529</v>
+        <v>77529.734609824969</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>5793.4973549606857</v>
+        <v>96686.389876169225</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>92324.135214834067</v>
+        <v>19483.676945575935</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>71903.961099807566</v>
+        <v>14458.000445741014</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>31247.132424581847</v>
+        <v>72959.661500398259</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>7140.9989546675542</v>
+        <v>268.75920192019896</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>16245.037851760968</v>
+        <v>60866.21135202438</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>75999.851270430532</v>
+        <v>27542.319249625736</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>74570.749666775926</v>
+        <v>46831.756035629078</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>27180.38478262732</v>
+        <v>24591.635843079395</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>39447.099908533222</v>
+        <v>46591.298376183957</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>71837.274693184518</v>
+        <v>26276.407927544977</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>47588.935158121392</v>
+        <v>14331.844020736262</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>89202.125817068139</v>
+        <v>61018.235746686711</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>74201.899809436087</v>
+        <v>27226.347251868454</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>62982.283687052288</v>
+        <v>30367.01849994955</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
         <f t="shared" ca="1" si="0"/>
-        <v>19759.336595891342</v>
+        <v>56205.168615184666</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
         <f t="shared" ref="A66:A129" ca="1" si="1">RAND()*100000</f>
-        <v>5023.5979277603592</v>
+        <v>38197.322418233729</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
         <f t="shared" ca="1" si="1"/>
-        <v>88270.677611084277</v>
+        <v>46281.485629846451</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
         <f t="shared" ca="1" si="1"/>
-        <v>21900.4416724765</v>
+        <v>26757.065145953031</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
         <f t="shared" ca="1" si="1"/>
-        <v>73449.32772596633</v>
+        <v>203.18652671560412</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
         <f t="shared" ca="1" si="1"/>
-        <v>66024.297007920337</v>
+        <v>82420.581119541937</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
         <f t="shared" ca="1" si="1"/>
-        <v>38832.628573907066</v>
+        <v>4766.0091280741553</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
         <f t="shared" ca="1" si="1"/>
-        <v>50700.523357190599</v>
+        <v>75570.254283306131</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
         <f t="shared" ca="1" si="1"/>
-        <v>10394.071548601192</v>
+        <v>73781.707249535888</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
         <f t="shared" ca="1" si="1"/>
-        <v>13335.79721860929</v>
+        <v>20320.961688111151</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
         <f t="shared" ca="1" si="1"/>
-        <v>75414.723481866444</v>
+        <v>43932.59608186558</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
         <f t="shared" ca="1" si="1"/>
-        <v>46193.820237065629</v>
+        <v>91107.596910041349</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
         <f t="shared" ca="1" si="1"/>
-        <v>21080.368228587566</v>
+        <v>19583.895867136402</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
         <f t="shared" ca="1" si="1"/>
-        <v>47143.131610089207</v>
+        <v>52957.318740064089</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
         <f t="shared" ca="1" si="1"/>
-        <v>32089.722411809296</v>
+        <v>11384.443251334309</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
         <f t="shared" ca="1" si="1"/>
-        <v>36667.085621055798</v>
+        <v>81202.237574899584</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
         <f t="shared" ca="1" si="1"/>
-        <v>29638.075165932121</v>
+        <v>40825.408043554526</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
         <f t="shared" ca="1" si="1"/>
-        <v>12363.653026935584</v>
+        <v>81741.511300356433</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83">
         <f t="shared" ca="1" si="1"/>
-        <v>61802.617095306232</v>
+        <v>35255.535882748016</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84">
         <f t="shared" ca="1" si="1"/>
-        <v>59383.51438151289</v>
+        <v>90771.003187537674</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
         <f t="shared" ca="1" si="1"/>
-        <v>74497.261264475892</v>
+        <v>14647.829874072439</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86">
         <f t="shared" ca="1" si="1"/>
-        <v>62906.795623027909</v>
+        <v>33784.148839080022</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87">
         <f t="shared" ca="1" si="1"/>
-        <v>25557.431501618845</v>
+        <v>29162.682617395007</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88">
         <f t="shared" ca="1" si="1"/>
-        <v>27578.698180971594</v>
+        <v>86094.095302848757</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89">
         <f t="shared" ca="1" si="1"/>
-        <v>91547.665800367424</v>
+        <v>28106.074568292337</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
         <f t="shared" ca="1" si="1"/>
-        <v>31733.300267124931</v>
+        <v>7556.5402526204025</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
         <f t="shared" ca="1" si="1"/>
-        <v>2887.2809292019297</v>
+        <v>66.153476405506069</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
         <f t="shared" ca="1" si="1"/>
-        <v>46739.075727364332</v>
+        <v>15742.833130322919</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
         <f t="shared" ca="1" si="1"/>
-        <v>47125.945962573409</v>
+        <v>77290.527952374294</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
         <f t="shared" ca="1" si="1"/>
-        <v>59613.650966973371</v>
+        <v>9787.7983772177595</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
         <f t="shared" ca="1" si="1"/>
-        <v>23857.624134916143</v>
+        <v>92703.547405107223</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
         <f t="shared" ca="1" si="1"/>
-        <v>27320.871243781075</v>
+        <v>87662.623112473564</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97">
         <f t="shared" ca="1" si="1"/>
-        <v>97354.248400160577</v>
+        <v>44391.735873738144</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
         <f t="shared" ca="1" si="1"/>
-        <v>30655.617000834001</v>
+        <v>5039.0680809934474</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
         <f t="shared" ca="1" si="1"/>
-        <v>69260.682475114561</v>
+        <v>53318.106065557382</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
         <f t="shared" ca="1" si="1"/>
-        <v>89358.458745210912</v>
+        <v>23232.067700702621</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
         <f t="shared" ca="1" si="1"/>
-        <v>63038.027579167385</v>
+        <v>96478.481916241086</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
         <f t="shared" ca="1" si="1"/>
-        <v>73071.292721691789</v>
+        <v>74674.93594243018</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
         <f t="shared" ca="1" si="1"/>
-        <v>97771.213704433074</v>
+        <v>87664.317293009459</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104">
         <f t="shared" ca="1" si="1"/>
-        <v>70609.839756684945</v>
+        <v>61567.158636473017</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
         <f t="shared" ca="1" si="1"/>
-        <v>16784.702230494309</v>
+        <v>83650.382199690532</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106">
         <f t="shared" ca="1" si="1"/>
-        <v>59508.684711116068</v>
+        <v>76393.247753923803</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107">
         <f t="shared" ca="1" si="1"/>
-        <v>34658.718931502575</v>
+        <v>99963.294810257357</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
         <f t="shared" ca="1" si="1"/>
-        <v>60085.549080842604</v>
+        <v>32726.46772360487</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
         <f t="shared" ca="1" si="1"/>
-        <v>31146.871632589533</v>
+        <v>6068.3400562081542</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
         <f t="shared" ca="1" si="1"/>
-        <v>74706.534529908822</v>
+        <v>32328.521627496022</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
         <f t="shared" ca="1" si="1"/>
-        <v>42277.015222192851</v>
+        <v>4361.3937635520124</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
         <f t="shared" ca="1" si="1"/>
-        <v>92641.059359553721</v>
+        <v>65455.839228814206</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113">
         <f t="shared" ca="1" si="1"/>
-        <v>35755.632759023705</v>
+        <v>61301.279611415172</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
         <f t="shared" ca="1" si="1"/>
-        <v>27989.336078878991</v>
+        <v>13334.175014844308</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115">
         <f t="shared" ca="1" si="1"/>
-        <v>27093.912451937751</v>
+        <v>34801.924745351665</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116">
         <f t="shared" ca="1" si="1"/>
-        <v>23603.742633264279</v>
+        <v>7051.2029223660729</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117">
         <f t="shared" ca="1" si="1"/>
-        <v>34717.172983650489</v>
+        <v>59926.88852639035</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118">
         <f t="shared" ca="1" si="1"/>
-        <v>11338.703275437179</v>
+        <v>95814.740656685855</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119">
         <f t="shared" ca="1" si="1"/>
-        <v>84995.951187386148</v>
+        <v>50731.091553082893</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120">
         <f t="shared" ca="1" si="1"/>
-        <v>11961.359666909033</v>
+        <v>97435.013296705263</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
         <f t="shared" ca="1" si="1"/>
-        <v>41121.453981453749</v>
+        <v>58201.579172537742</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122">
         <f t="shared" ca="1" si="1"/>
-        <v>70915.946469160772</v>
+        <v>77343.452057993054</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123">
         <f t="shared" ca="1" si="1"/>
-        <v>81563.16528214654</v>
+        <v>62718.022975781663</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124">
         <f t="shared" ca="1" si="1"/>
-        <v>20169.033695483442</v>
+        <v>34778.924791033918</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125">
         <f t="shared" ca="1" si="1"/>
-        <v>19819.672376202514</v>
+        <v>37256.815437776182</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126">
         <f t="shared" ca="1" si="1"/>
-        <v>48467.622325935823</v>
+        <v>82379.410965469695</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127">
         <f t="shared" ca="1" si="1"/>
-        <v>35975.148880275454</v>
+        <v>69803.127822208</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128">
         <f t="shared" ca="1" si="1"/>
-        <v>45038.540944818218</v>
+        <v>19170.936424110772</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129">
         <f t="shared" ca="1" si="1"/>
-        <v>32274.432609184467</v>
+        <v>55725.666049161271</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130">
         <f t="shared" ref="A130:A193" ca="1" si="2">RAND()*100000</f>
-        <v>71460.696929300713</v>
+        <v>46327.765562278211</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131">
         <f t="shared" ca="1" si="2"/>
-        <v>47592.230158171202</v>
+        <v>39977.693824353431</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132">
         <f t="shared" ca="1" si="2"/>
-        <v>10098.752136715328</v>
+        <v>97647.297498804313</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133">
         <f t="shared" ca="1" si="2"/>
-        <v>9515.0130039749474</v>
+        <v>90964.550412592187</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134">
         <f t="shared" ca="1" si="2"/>
-        <v>15116.483226579092</v>
+        <v>55914.297086804763</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135">
         <f t="shared" ca="1" si="2"/>
-        <v>28119.716741436485</v>
+        <v>6567.5197984324532</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136">
         <f t="shared" ca="1" si="2"/>
-        <v>22690.903060116441</v>
+        <v>52919.75432352112</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137">
         <f t="shared" ca="1" si="2"/>
-        <v>1947.8959759569036</v>
+        <v>50005.429240654732</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138">
         <f t="shared" ca="1" si="2"/>
-        <v>59283.559536037908</v>
+        <v>1927.6157809046902</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139">
         <f t="shared" ca="1" si="2"/>
-        <v>40030.999514745847</v>
+        <v>28204.598082144461</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140">
         <f t="shared" ca="1" si="2"/>
-        <v>40135.41394428529</v>
+        <v>79639.035843274323</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141">
         <f t="shared" ca="1" si="2"/>
-        <v>77740.784776182205</v>
+        <v>95590.7438042172</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
         <f t="shared" ca="1" si="2"/>
-        <v>85062.503135255072</v>
+        <v>66742.386791713565</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
         <f t="shared" ca="1" si="2"/>
-        <v>59363.801262082328</v>
+        <v>735.18909471282927</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144">
         <f t="shared" ca="1" si="2"/>
-        <v>49317.720229008621</v>
+        <v>52869.137843202843</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145">
         <f t="shared" ca="1" si="2"/>
-        <v>36867.137868865961</v>
+        <v>16323.243463830406</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146">
         <f t="shared" ca="1" si="2"/>
-        <v>60554.027357192805</v>
+        <v>38333.916528711597</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147">
         <f t="shared" ca="1" si="2"/>
-        <v>60099.163677235221</v>
+        <v>25009.663137959549</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148">
         <f t="shared" ca="1" si="2"/>
-        <v>52993.505354111083</v>
+        <v>7968.9904353341335</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
         <f t="shared" ca="1" si="2"/>
-        <v>37127.249025474608</v>
+        <v>84056.389617010092</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150">
         <f t="shared" ca="1" si="2"/>
-        <v>20281.066705347461</v>
+        <v>36259.762869130376</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151">
         <f t="shared" ca="1" si="2"/>
-        <v>93212.159632973722</v>
+        <v>15101.85785527277</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
         <f t="shared" ca="1" si="2"/>
-        <v>52091.650934552999</v>
+        <v>7074.2821012208187</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153">
         <f t="shared" ca="1" si="2"/>
-        <v>1744.4788106253827</v>
+        <v>31176.433574168972</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
         <f t="shared" ca="1" si="2"/>
-        <v>31861.306436417246</v>
+        <v>4849.7669723396421</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155">
         <f t="shared" ca="1" si="2"/>
-        <v>32056.927456000951</v>
+        <v>44705.170299102239</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156">
         <f t="shared" ca="1" si="2"/>
-        <v>85189.159308275746</v>
+        <v>31854.872950544323</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157">
         <f t="shared" ca="1" si="2"/>
-        <v>88439.630685685028</v>
+        <v>75316.501090324877</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158">
         <f t="shared" ca="1" si="2"/>
-        <v>15571.543108148046</v>
+        <v>47305.766229381443</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159">
         <f t="shared" ca="1" si="2"/>
-        <v>71758.327533975607</v>
+        <v>10454.42187794985</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160">
         <f t="shared" ca="1" si="2"/>
-        <v>4548.4610797014266</v>
+        <v>55490.240350410539</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161">
         <f t="shared" ca="1" si="2"/>
-        <v>25593.292857250428</v>
+        <v>47942.365764463531</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162">
         <f t="shared" ca="1" si="2"/>
-        <v>44757.71334618995</v>
+        <v>40387.265110563894</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163">
         <f t="shared" ca="1" si="2"/>
-        <v>12355.697151684908</v>
+        <v>5544.0660143567857</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164">
         <f t="shared" ca="1" si="2"/>
-        <v>29143.902688326052</v>
+        <v>7470.7917753313759</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165">
         <f t="shared" ca="1" si="2"/>
-        <v>47104.567896375396</v>
+        <v>88212.627120002013</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166">
         <f t="shared" ca="1" si="2"/>
-        <v>87768.035005414509</v>
+        <v>23794.90750555804</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167">
         <f t="shared" ca="1" si="2"/>
-        <v>37191.772185299233</v>
+        <v>27180.973807199571</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168">
         <f t="shared" ca="1" si="2"/>
-        <v>52081.530561456282</v>
+        <v>61718.612861184876</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169">
         <f t="shared" ca="1" si="2"/>
-        <v>26112.872870479008</v>
+        <v>89434.151644814207</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170">
         <f t="shared" ca="1" si="2"/>
-        <v>95694.182932231823</v>
+        <v>20671.319510272911</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171">
         <f t="shared" ca="1" si="2"/>
-        <v>38686.937770711171</v>
+        <v>16406.925775960048</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
         <f t="shared" ca="1" si="2"/>
-        <v>99524.01069405803</v>
+        <v>87468.033124493944</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
         <f t="shared" ca="1" si="2"/>
-        <v>10374.220203409657</v>
+        <v>29926.269076568336</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174">
         <f t="shared" ca="1" si="2"/>
-        <v>65374.581853674783</v>
+        <v>3698.6189420991632</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
         <f t="shared" ca="1" si="2"/>
-        <v>82471.00296064846</v>
+        <v>19271.20854157205</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
         <f t="shared" ca="1" si="2"/>
-        <v>41266.671787064261</v>
+        <v>60066.722240309078</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177">
         <f t="shared" ca="1" si="2"/>
-        <v>95117.946604726822</v>
+        <v>45891.346615661307</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178">
         <f t="shared" ca="1" si="2"/>
-        <v>53860.620590102037</v>
+        <v>88925.310905461345</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179">
         <f t="shared" ca="1" si="2"/>
-        <v>60632.26210553453</v>
+        <v>63373.391128333453</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180">
         <f t="shared" ca="1" si="2"/>
-        <v>52114.923344199349</v>
+        <v>92929.151226786373</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181">
         <f t="shared" ca="1" si="2"/>
-        <v>36370.161466917118</v>
+        <v>71146.098907269377</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182">
         <f t="shared" ca="1" si="2"/>
-        <v>83461.577155299587</v>
+        <v>747.28337854874644</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183">
         <f t="shared" ca="1" si="2"/>
-        <v>15573.794978998578</v>
+        <v>96446.116684465247</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184">
         <f t="shared" ca="1" si="2"/>
-        <v>41651.353741527884</v>
+        <v>41076.53946797036</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185">
         <f t="shared" ca="1" si="2"/>
-        <v>7374.6031808186954</v>
+        <v>72840.470809168357</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186">
         <f t="shared" ca="1" si="2"/>
-        <v>53923.246956103343</v>
+        <v>3862.931596819963</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
         <f t="shared" ca="1" si="2"/>
-        <v>74645.807946216402</v>
+        <v>14013.208095579943</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188">
         <f t="shared" ca="1" si="2"/>
-        <v>98765.137763113511</v>
+        <v>29500.999551620833</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189">
         <f t="shared" ca="1" si="2"/>
-        <v>47781.29195254873</v>
+        <v>47472.101521049612</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190">
         <f t="shared" ca="1" si="2"/>
-        <v>16146.14577966682</v>
+        <v>91384.526960225703</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191">
         <f t="shared" ca="1" si="2"/>
-        <v>33892.284385592982</v>
+        <v>30812.750659734545</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192">
         <f t="shared" ca="1" si="2"/>
-        <v>4866.8138053417078</v>
+        <v>31275.106651841645</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
         <f t="shared" ca="1" si="2"/>
-        <v>93812.389425264293</v>
+        <v>57165.084858418282</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194">
         <f t="shared" ref="A194:A257" ca="1" si="3">RAND()*100000</f>
-        <v>40473.843280874957</v>
+        <v>74216.011635493705</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195">
         <f t="shared" ca="1" si="3"/>
-        <v>45508.347912013211</v>
+        <v>31184.651549288588</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196">
         <f t="shared" ca="1" si="3"/>
-        <v>88926.168216246442</v>
+        <v>60026.949312723664</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197">
         <f t="shared" ca="1" si="3"/>
-        <v>27543.834652965128</v>
+        <v>15806.791050357006</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198">
         <f t="shared" ca="1" si="3"/>
-        <v>83018.699797347188</v>
+        <v>74452.985589602598</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199">
         <f t="shared" ca="1" si="3"/>
-        <v>69030.796280207724</v>
+        <v>10655.565072444984</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200">
         <f t="shared" ca="1" si="3"/>
-        <v>8747.8954644991445</v>
+        <v>86756.032205295152</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
         <f t="shared" ca="1" si="3"/>
-        <v>21371.533750014747</v>
+        <v>74879.118875465007</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
         <f t="shared" ca="1" si="3"/>
-        <v>21295.941696017129</v>
+        <v>53811.874768664944</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
         <f t="shared" ca="1" si="3"/>
-        <v>24659.417746234802</v>
+        <v>20009.958689077823</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204">
         <f t="shared" ca="1" si="3"/>
-        <v>43093.671448195761</v>
+        <v>68626.121507534859</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205">
         <f t="shared" ca="1" si="3"/>
-        <v>88120.271139716235</v>
+        <v>27137.505238233538</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
         <f t="shared" ca="1" si="3"/>
-        <v>67424.93693497809</v>
+        <v>98675.162026735459</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
         <f t="shared" ca="1" si="3"/>
-        <v>61821.987353355842</v>
+        <v>93221.573016730981</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
         <f t="shared" ca="1" si="3"/>
-        <v>7564.5262380511276</v>
+        <v>39038.08400745671</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
         <f t="shared" ca="1" si="3"/>
-        <v>98821.469230371324</v>
+        <v>84891.442700318483</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210">
         <f t="shared" ca="1" si="3"/>
-        <v>57041.972148772693</v>
+        <v>38112.747533240086</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211">
         <f t="shared" ca="1" si="3"/>
-        <v>99846.967660823677</v>
+        <v>85217.15391882768</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212">
         <f t="shared" ca="1" si="3"/>
-        <v>81283.517518576482</v>
+        <v>69955.191832856668</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213">
         <f t="shared" ca="1" si="3"/>
-        <v>44894.206336468756</v>
+        <v>32272.233421035835</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214">
         <f t="shared" ca="1" si="3"/>
-        <v>13831.31293244454</v>
+        <v>86734.241529661813</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215">
         <f t="shared" ca="1" si="3"/>
-        <v>82373.895036309477</v>
+        <v>13929.297633674087</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
         <f t="shared" ca="1" si="3"/>
-        <v>3449.5932341941484</v>
+        <v>52004.930069606635</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217">
         <f t="shared" ca="1" si="3"/>
-        <v>98833.409730649262</v>
+        <v>79315.672045696629</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218">
         <f t="shared" ca="1" si="3"/>
-        <v>45166.64378330257</v>
+        <v>76534.678944423766</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219">
         <f t="shared" ca="1" si="3"/>
-        <v>66854.350343202474</v>
+        <v>60328.067794234441</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220">
         <f t="shared" ca="1" si="3"/>
-        <v>25115.541652570893</v>
+        <v>54569.420184724047</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221">
         <f t="shared" ca="1" si="3"/>
-        <v>42081.109151212571</v>
+        <v>96594.332743641295</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
         <f t="shared" ca="1" si="3"/>
-        <v>74366.244453380743</v>
+        <v>62806.781723527383</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
         <f t="shared" ca="1" si="3"/>
-        <v>90788.29790639109</v>
+        <v>17607.875565014554</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224">
         <f t="shared" ca="1" si="3"/>
-        <v>80184.557704207284</v>
+        <v>82126.121118034978</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225">
         <f t="shared" ca="1" si="3"/>
-        <v>26370.992774296021</v>
+        <v>52467.188828277336</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226">
         <f t="shared" ca="1" si="3"/>
-        <v>15288.934351005955</v>
+        <v>47223.126485468456</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227">
         <f t="shared" ca="1" si="3"/>
-        <v>38062.567842745855</v>
+        <v>18537.557503741566</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228">
         <f t="shared" ca="1" si="3"/>
-        <v>52701.332375954276</v>
+        <v>9458.4447752564811</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229">
         <f t="shared" ca="1" si="3"/>
-        <v>74315.623574975165</v>
+        <v>88470.184056297847</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230">
         <f t="shared" ca="1" si="3"/>
-        <v>3274.148463019977</v>
+        <v>47331.424894504838</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
         <f t="shared" ca="1" si="3"/>
-        <v>56114.0486722571</v>
+        <v>72122.327278959478</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232">
         <f t="shared" ca="1" si="3"/>
-        <v>92823.252242840317</v>
+        <v>82832.999785003019</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233">
         <f t="shared" ca="1" si="3"/>
-        <v>87344.640742160453</v>
+        <v>21589.153571911003</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234">
         <f t="shared" ca="1" si="3"/>
-        <v>49891.773695444754</v>
+        <v>52756.01047567647</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235">
         <f t="shared" ca="1" si="3"/>
-        <v>55004.614031923746</v>
+        <v>20929.760033220136</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
         <f t="shared" ca="1" si="3"/>
-        <v>1144.5812547203338</v>
+        <v>95968.911984120758</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
         <f t="shared" ca="1" si="3"/>
-        <v>88260.594313048729</v>
+        <v>16.573202267800013</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238">
         <f t="shared" ca="1" si="3"/>
-        <v>58329.525983837448</v>
+        <v>35148.931337254697</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239">
         <f t="shared" ca="1" si="3"/>
-        <v>30062.102877693174</v>
+        <v>16692.728146544567</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240">
         <f t="shared" ca="1" si="3"/>
-        <v>46835.173125487818</v>
+        <v>16767.443478913901</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241">
         <f t="shared" ca="1" si="3"/>
-        <v>31443.338107743137</v>
+        <v>56391.084336897366</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242">
         <f t="shared" ca="1" si="3"/>
-        <v>76273.649897558716</v>
+        <v>35555.692916778062</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243">
         <f t="shared" ca="1" si="3"/>
-        <v>67485.031207166685</v>
+        <v>72168.067923657887</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244">
         <f t="shared" ca="1" si="3"/>
-        <v>50448.504050462536</v>
+        <v>79698.584547461243</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245">
         <f t="shared" ca="1" si="3"/>
-        <v>78889.080566569421</v>
+        <v>43688.529392388409</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246">
         <f t="shared" ca="1" si="3"/>
-        <v>88264.230111877347</v>
+        <v>95326.558968462952</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247">
         <f t="shared" ca="1" si="3"/>
-        <v>94265.480567292383</v>
+        <v>91856.748068464265</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248">
         <f t="shared" ca="1" si="3"/>
-        <v>84592.351540940901</v>
+        <v>49544.888338574303</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249">
         <f t="shared" ca="1" si="3"/>
-        <v>94510.592983100592</v>
+        <v>61662.930984360057</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250">
         <f t="shared" ca="1" si="3"/>
-        <v>2263.9313460199542</v>
+        <v>85780.382218902596</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
         <f t="shared" ca="1" si="3"/>
-        <v>58279.061209213476</v>
+        <v>44368.481815914471</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252">
         <f t="shared" ca="1" si="3"/>
-        <v>66411.77786080855</v>
+        <v>15413.787415075119</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253">
         <f t="shared" ca="1" si="3"/>
-        <v>50790.641420776657</v>
+        <v>3866.128725021445</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254">
         <f t="shared" ca="1" si="3"/>
-        <v>47434.294228852355</v>
+        <v>93833.641652970546</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
         <f t="shared" ca="1" si="3"/>
-        <v>72619.523042830217</v>
+        <v>86556.453896077073</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
         <f t="shared" ca="1" si="3"/>
-        <v>62127.913175509289</v>
+        <v>21281.696601951484</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257">
         <f t="shared" ca="1" si="3"/>
-        <v>87546.000853813908</v>
+        <v>60393.585341113132</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258">
         <f t="shared" ref="A258:A300" ca="1" si="4">RAND()*100000</f>
-        <v>21628.169714807267</v>
+        <v>9631.4710727985585</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259">
         <f t="shared" ca="1" si="4"/>
-        <v>7661.289758644818</v>
+        <v>81436.0523498564</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260">
         <f t="shared" ca="1" si="4"/>
-        <v>80376.132007350403</v>
+        <v>64810.277921736102</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
         <f t="shared" ca="1" si="4"/>
-        <v>49119.243829983796</v>
+        <v>80796.855761485611</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262">
         <f t="shared" ca="1" si="4"/>
-        <v>62565.766621205177</v>
+        <v>81699.501218464939</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263">
         <f t="shared" ca="1" si="4"/>
-        <v>32645.468408949764</v>
+        <v>67628.696598891926</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264">
         <f t="shared" ca="1" si="4"/>
-        <v>29527.887313225408</v>
+        <v>92481.565309964877</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265">
         <f t="shared" ca="1" si="4"/>
-        <v>37855.119366929292</v>
+        <v>20660.375560039134</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
         <f t="shared" ca="1" si="4"/>
-        <v>20157.731024740344</v>
+        <v>26563.017690734512</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
         <f t="shared" ca="1" si="4"/>
-        <v>53383.598154193132</v>
+        <v>55687.209935687744</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268">
         <f t="shared" ca="1" si="4"/>
-        <v>44292.885815233341</v>
+        <v>3758.7324053926509</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269">
         <f t="shared" ca="1" si="4"/>
-        <v>75687.386324179402</v>
+        <v>49850.179184218658</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270">
         <f t="shared" ca="1" si="4"/>
-        <v>7296.8279052664457</v>
+        <v>82743.568572223405</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271">
         <f t="shared" ca="1" si="4"/>
-        <v>78601.46607767079</v>
+        <v>75489.632172439771</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272">
         <f t="shared" ca="1" si="4"/>
-        <v>12661.960764177116</v>
+        <v>99742.498359389938</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273">
         <f t="shared" ca="1" si="4"/>
-        <v>77363.312422157178</v>
+        <v>53846.024022825848</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274">
         <f t="shared" ca="1" si="4"/>
-        <v>61671.83062234828</v>
+        <v>63890.940661931294</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275">
         <f t="shared" ca="1" si="4"/>
-        <v>20394.390434520115</v>
+        <v>88367.534719464558</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276">
         <f t="shared" ca="1" si="4"/>
-        <v>63718.267382029568</v>
+        <v>20940.266673113139</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277">
         <f t="shared" ca="1" si="4"/>
-        <v>21124.627175533784</v>
+        <v>7889.9701348819071</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278">
         <f t="shared" ca="1" si="4"/>
-        <v>29691.429854227692</v>
+        <v>1562.0479445477952</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279">
         <f t="shared" ca="1" si="4"/>
-        <v>55780.692122471068</v>
+        <v>15768.973018908406</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
         <f t="shared" ca="1" si="4"/>
-        <v>83235.757526520698</v>
+        <v>73734.695119454336</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281">
         <f t="shared" ca="1" si="4"/>
-        <v>27432.05677732492</v>
+        <v>27764.513541795422</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282">
         <f t="shared" ca="1" si="4"/>
-        <v>44926.705480911653</v>
+        <v>27513.671107487124</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283">
         <f t="shared" ca="1" si="4"/>
-        <v>73757.963393410959</v>
+        <v>85398.26286365783</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284">
         <f t="shared" ca="1" si="4"/>
-        <v>44376.240533009513</v>
+        <v>70004.184749920751</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285">
         <f t="shared" ca="1" si="4"/>
-        <v>74844.270489113114</v>
+        <v>70162.178060022517</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286">
         <f t="shared" ca="1" si="4"/>
-        <v>11667.567375848676</v>
+        <v>36993.252620979678</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287">
         <f t="shared" ca="1" si="4"/>
-        <v>54988.804978767177</v>
+        <v>80316.152332030397</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288">
         <f t="shared" ca="1" si="4"/>
-        <v>22721.771159191638</v>
+        <v>79151.537106832053</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289">
         <f t="shared" ca="1" si="4"/>
-        <v>16393.90934291438</v>
+        <v>80695.892563418776</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290">
         <f t="shared" ca="1" si="4"/>
-        <v>1643.0797805726095</v>
+        <v>60141.984108483441</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291">
         <f t="shared" ca="1" si="4"/>
-        <v>32715.013909009005</v>
+        <v>35278.419403375796</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292">
         <f t="shared" ca="1" si="4"/>
-        <v>70696.334537307397</v>
+        <v>2415.4843877974731</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293">
         <f t="shared" ca="1" si="4"/>
-        <v>45992.742624846083</v>
+        <v>1121.7805640474699</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294">
         <f t="shared" ca="1" si="4"/>
-        <v>80025.748370964095</v>
+        <v>89029.145256212738</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295">
         <f t="shared" ca="1" si="4"/>
-        <v>16536.174184590203</v>
+        <v>37036.700113074716</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296">
         <f t="shared" ca="1" si="4"/>
-        <v>93006.332033772997</v>
+        <v>66203.165796158908</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297">
         <f t="shared" ca="1" si="4"/>
-        <v>31846.59277236327</v>
+        <v>95394.28627016356</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298">
         <f t="shared" ca="1" si="4"/>
-        <v>8818.722297507109</v>
+        <v>33774.564724181888</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299">
         <f t="shared" ca="1" si="4"/>
-        <v>25305.685140810696</v>
+        <v>25625.270628414208</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300">
         <f t="shared" ca="1" si="4"/>
-        <v>38720.707318238812</v>
+        <v>75395.000477534733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Base de datos invitados separar primos
</commit_message>
<xml_diff>
--- a/src/assets/data/BD_INVITADOS.xlsx
+++ b/src/assets/data/BD_INVITADOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Claudia Documentos\CYB\proyectos\angular\AppWedding\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFF37E7D-EE9B-4A3D-AD95-D8E23616471C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5711DF1A-B574-40FA-BF6B-CD94FE3F0284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="140">
   <si>
     <t>invitado</t>
   </si>
@@ -443,6 +443,24 @@
   </si>
   <si>
     <t>BC0000060</t>
+  </si>
+  <si>
+    <t>Marco Antonio Fernandez Barboza</t>
+  </si>
+  <si>
+    <t>BC0000061</t>
+  </si>
+  <si>
+    <t>Lyly Romina Fernandez Barboza</t>
+  </si>
+  <si>
+    <t>BC0000062</t>
+  </si>
+  <si>
+    <t>Mavila Yesenia Fernandez Barboza</t>
+  </si>
+  <si>
+    <t>BC0000063</t>
   </si>
 </sst>
 </file>
@@ -831,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2953,7 +2971,7 @@
         <v>2</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" ref="C61" si="18">CONCATENATE(E61,F61)</f>
+        <f t="shared" ref="C61:C62" si="18">CONCATENATE(E61,F61)</f>
         <v>BC000006044300</v>
       </c>
       <c r="D61">
@@ -2970,13 +2988,118 @@
         <v>12</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" ref="H61" si="19">CONCATENATE(G61,C61)</f>
+        <f t="shared" ref="H61:H62" si="19">CONCATENATE(G61,C61)</f>
         <v>https://bvasquez-code.github.io/AppWedding/?id=BC000006044300</v>
       </c>
       <c r="I61" t="s">
         <v>36</v>
       </c>
       <c r="J61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="18"/>
+        <v>BC000006110415</v>
+      </c>
+      <c r="D62">
+        <v>968238273</v>
+      </c>
+      <c r="E62" t="s">
+        <v>135</v>
+      </c>
+      <c r="F62">
+        <f>Hoja2!B62</f>
+        <v>10415</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="19"/>
+        <v>https://bvasquez-code.github.io/AppWedding/?id=BC000006110415</v>
+      </c>
+      <c r="I62" t="s">
+        <v>36</v>
+      </c>
+      <c r="J62" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" ref="C63:C64" si="20">CONCATENATE(E63,F63)</f>
+        <v>BC000006261425</v>
+      </c>
+      <c r="D63">
+        <v>968238274</v>
+      </c>
+      <c r="E63" t="s">
+        <v>137</v>
+      </c>
+      <c r="F63">
+        <f>Hoja2!B63</f>
+        <v>61425</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" ref="H63:H64" si="21">CONCATENATE(G63,C63)</f>
+        <v>https://bvasquez-code.github.io/AppWedding/?id=BC000006261425</v>
+      </c>
+      <c r="I63" t="s">
+        <v>36</v>
+      </c>
+      <c r="J63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="20"/>
+        <v>BC000006382687</v>
+      </c>
+      <c r="D64">
+        <v>968238275</v>
+      </c>
+      <c r="E64" t="s">
+        <v>139</v>
+      </c>
+      <c r="F64">
+        <f>Hoja2!B64</f>
+        <v>82687</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="21"/>
+        <v>https://bvasquez-code.github.io/AppWedding/?id=BC000006382687</v>
+      </c>
+      <c r="I64" t="s">
+        <v>36</v>
+      </c>
+      <c r="J64" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2994,9 +3117,13 @@
     <hyperlink ref="G59" r:id="rId8" xr:uid="{E8E5DF5A-BD83-41C6-A0D4-F60E9E4A8E7C}"/>
     <hyperlink ref="G60" r:id="rId9" xr:uid="{7E79577C-6EF6-4147-8ADD-CAA43C1568B0}"/>
     <hyperlink ref="G61" r:id="rId10" xr:uid="{D6085AE8-AD19-4176-9046-080BB6F63E97}"/>
+    <hyperlink ref="G62" r:id="rId11" xr:uid="{53CA40E2-B834-4047-9A4F-07DF18F0EA8D}"/>
+    <hyperlink ref="G64" r:id="rId12" xr:uid="{8988C9C0-0A7A-489A-B45E-8848CF69343E}"/>
+    <hyperlink ref="G63" r:id="rId13" xr:uid="{E6DF134E-C693-4EE7-B86F-D64F94589410}"/>
+    <hyperlink ref="G64" r:id="rId14" xr:uid="{843126AE-3780-43F8-8F5E-AF20EE8FF32E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -5729,1801 +5856,1801 @@
     <row r="1" spans="1:1">
       <c r="A1">
         <f ca="1">RAND()*100000</f>
-        <v>23762.775885489518</v>
+        <v>56693.028327795182</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
         <f t="shared" ref="A2:A65" ca="1" si="0">RAND()*100000</f>
-        <v>85562.368421791951</v>
+        <v>96933.958859940845</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>1555.36391708887</v>
+        <v>29783.252155305585</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>14919.735001759926</v>
+        <v>15639.905486014572</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>81269.301862069697</v>
+        <v>72879.003952455867</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>85373.612136930096</v>
+        <v>9816.1808730444882</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>4113.4359900185882</v>
+        <v>12876.83131340145</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>49776.364896016079</v>
+        <v>46652.30331411834</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>87109.617352486064</v>
+        <v>17403.019531403887</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>43120.012173828945</v>
+        <v>56417.578684572021</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>37195.155699922288</v>
+        <v>50283.440904430856</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>83344.958136466244</v>
+        <v>73015.464733939443</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>81916.496946473286</v>
+        <v>72315.456158886533</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>72544.10245145543</v>
+        <v>2100.8057815362081</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>48245.556068945159</v>
+        <v>96106.824295366532</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>62241.593004814174</v>
+        <v>55658.4355727722</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>17473.206697265643</v>
+        <v>3679.5030190140965</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>77399.414054874011</v>
+        <v>34701.015544074413</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
         <f ca="1">RAND()*100000</f>
-        <v>9209.7807779920167</v>
+        <v>50491.267483226722</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>53549.326607981588</v>
+        <v>37298.922850269679</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>1514.3890670996973</v>
+        <v>12276.818267545974</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>69882.692309905207</v>
+        <v>54159.355153896002</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>12512.877865482507</v>
+        <v>52331.782792911741</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>49444.514844482001</v>
+        <v>17763.730318651949</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>60180.004322410321</v>
+        <v>20714.896740541801</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>8129.2139884443613</v>
+        <v>49999.542205790938</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>14026.366061620132</v>
+        <v>41233.42516576971</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>79940.091921460771</v>
+        <v>11315.8677898198</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>83773.562091667904</v>
+        <v>39059.048706929869</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>52274.862666113208</v>
+        <v>9721.6261614477935</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>85650.226677632483</v>
+        <v>12699.191271746568</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>12231.852439481527</v>
+        <v>80693.030452416089</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>71616.869148189435</v>
+        <v>90746.619170819729</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>83367.614786722988</v>
+        <v>29383.772920546548</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>90774.975858755191</v>
+        <v>53521.799653954215</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>60068.682127626402</v>
+        <v>30637.391588218608</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>32231.752590640128</v>
+        <v>51578.752319888408</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>27350.796687072852</v>
+        <v>82306.574638927079</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>56178.814508681295</v>
+        <v>55730.831652952438</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>17946.775689191007</v>
+        <v>74375.036799215086</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>86550.680146894068</v>
+        <v>96396.559634064237</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>23371.748573898942</v>
+        <v>94131.569963068745</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>6900.0881419622792</v>
+        <v>2099.6609717676697</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>98438.987965151231</v>
+        <v>61006.480128646777</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>19584.692218429856</v>
+        <v>70084.47429296498</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>29281.026268124799</v>
+        <v>90947.87248573071</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>81712.005596741452</v>
+        <v>96049.8266890503</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>82004.777748061548</v>
+        <v>14364.685876241245</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>285.52374274133376</v>
+        <v>29849.534797852662</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>80514.844513116041</v>
+        <v>71198.753145375638</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>34510.317202935817</v>
+        <v>129.38272545445218</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>65403.026010204914</v>
+        <v>46998.089912148454</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>47989.772785801688</v>
+        <v>40830.816515521365</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>54883.557667783854</v>
+        <v>94523.417059350366</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>24463.39245889262</v>
+        <v>63564.423542581397</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>98351.368454878408</v>
+        <v>80140.755364530138</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>51034.843781766227</v>
+        <v>42034.796363760943</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>33078.052263477264</v>
+        <v>78493.790432303897</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>37243.343858897249</v>
+        <v>19188.767650709306</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>42396.834058416855</v>
+        <v>82519.332185453357</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>45778.469855942494</v>
+        <v>70695.691717334485</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>22622.88753424192</v>
+        <v>32178.104585106048</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>60218.124458299106</v>
+        <v>33664.969472599274</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>72120.962689890774</v>
+        <v>64233.539907602164</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
         <f t="shared" ca="1" si="0"/>
-        <v>62202.838081121678</v>
+        <v>8931.6102746055385</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
         <f t="shared" ref="A66:A129" ca="1" si="1">RAND()*100000</f>
-        <v>5011.7883177351105</v>
+        <v>86184.969543427243</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
         <f t="shared" ca="1" si="1"/>
-        <v>84193.835871779869</v>
+        <v>15809.887183622985</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
         <f t="shared" ca="1" si="1"/>
-        <v>89161.213565273749</v>
+        <v>67188.403082868303</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
         <f t="shared" ca="1" si="1"/>
-        <v>61597.997255415183</v>
+        <v>97670.54622079953</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
         <f t="shared" ca="1" si="1"/>
-        <v>60514.48709383994</v>
+        <v>70057.888077221083</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
         <f t="shared" ca="1" si="1"/>
-        <v>66838.469292929673</v>
+        <v>82915.630236072495</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
         <f t="shared" ca="1" si="1"/>
-        <v>94825.845772372399</v>
+        <v>2350.4657038213918</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
         <f t="shared" ca="1" si="1"/>
-        <v>83563.608030365853</v>
+        <v>86241.863492894103</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
         <f t="shared" ca="1" si="1"/>
-        <v>79707.374193624419</v>
+        <v>16734.261342593949</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
         <f t="shared" ca="1" si="1"/>
-        <v>44816.520364373493</v>
+        <v>47288.319521176672</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
         <f t="shared" ca="1" si="1"/>
-        <v>19787.917317644089</v>
+        <v>34681.739939602208</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
         <f t="shared" ca="1" si="1"/>
-        <v>86860.346525992398</v>
+        <v>53544.383442732709</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
         <f t="shared" ca="1" si="1"/>
-        <v>7406.0362570150028</v>
+        <v>86444.197528884411</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
         <f t="shared" ca="1" si="1"/>
-        <v>67258.099484247985</v>
+        <v>62668.331330790294</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
         <f t="shared" ca="1" si="1"/>
-        <v>19940.67819872556</v>
+        <v>30976.667777743583</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
         <f t="shared" ca="1" si="1"/>
-        <v>7714.3805689605551</v>
+        <v>13365.105000791655</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
         <f t="shared" ca="1" si="1"/>
-        <v>1548.3742835022517</v>
+        <v>62847.209784213766</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83">
         <f t="shared" ca="1" si="1"/>
-        <v>63047.062263660613</v>
+        <v>64766.972113461918</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84">
         <f t="shared" ca="1" si="1"/>
-        <v>57583.319866728765</v>
+        <v>99385.043009097557</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
         <f t="shared" ca="1" si="1"/>
-        <v>25636.626720101176</v>
+        <v>24179.601330763366</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86">
         <f t="shared" ca="1" si="1"/>
-        <v>27230.690337867436</v>
+        <v>84328.388648445005</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87">
         <f t="shared" ca="1" si="1"/>
-        <v>35329.787389506164</v>
+        <v>24927.878476712052</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88">
         <f t="shared" ca="1" si="1"/>
-        <v>96582.486755819118</v>
+        <v>3104.8276435636344</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89">
         <f t="shared" ca="1" si="1"/>
-        <v>54769.161773121254</v>
+        <v>85570.863274360483</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
         <f t="shared" ca="1" si="1"/>
-        <v>71599.128972448205</v>
+        <v>98344.003767708637</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
         <f t="shared" ca="1" si="1"/>
-        <v>70728.437473433311</v>
+        <v>2875.0925258041125</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
         <f t="shared" ca="1" si="1"/>
-        <v>6040.7148388862515</v>
+        <v>55806.155794194543</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
         <f t="shared" ca="1" si="1"/>
-        <v>83396.897704371877</v>
+        <v>57006.179482361396</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
         <f t="shared" ca="1" si="1"/>
-        <v>24362.738444156883</v>
+        <v>85195.275397785241</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
         <f t="shared" ca="1" si="1"/>
-        <v>74351.029081698172</v>
+        <v>77452.990215667087</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
         <f t="shared" ca="1" si="1"/>
-        <v>25486.819238628301</v>
+        <v>86900.546703865504</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97">
         <f t="shared" ca="1" si="1"/>
-        <v>25511.231108086053</v>
+        <v>1016.4969243281696</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
         <f t="shared" ca="1" si="1"/>
-        <v>54685.764065591982</v>
+        <v>19570.32859686928</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
         <f t="shared" ca="1" si="1"/>
-        <v>48293.438123325839</v>
+        <v>44520.617110192048</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
         <f t="shared" ca="1" si="1"/>
-        <v>74745.052507320215</v>
+        <v>94034.569325711651</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
         <f t="shared" ca="1" si="1"/>
-        <v>75906.330776320072</v>
+        <v>67143.280480517817</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
         <f t="shared" ca="1" si="1"/>
-        <v>24300.910105137642</v>
+        <v>14537.942538389425</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
         <f t="shared" ca="1" si="1"/>
-        <v>99591.94485247659</v>
+        <v>60154.527990988725</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104">
         <f t="shared" ca="1" si="1"/>
-        <v>70434.000608582704</v>
+        <v>98569.301583961438</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
         <f t="shared" ca="1" si="1"/>
-        <v>51433.531036597255</v>
+        <v>5824.1761876812288</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106">
         <f t="shared" ca="1" si="1"/>
-        <v>74481.173558892435</v>
+        <v>48171.655577759295</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107">
         <f t="shared" ca="1" si="1"/>
-        <v>48876.145734645892</v>
+        <v>94840.503327622209</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
         <f t="shared" ca="1" si="1"/>
-        <v>71241.430319973209</v>
+        <v>30565.165158281026</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
         <f t="shared" ca="1" si="1"/>
-        <v>2874.5778375275477</v>
+        <v>21696.192394214519</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
         <f t="shared" ca="1" si="1"/>
-        <v>39773.14730728521</v>
+        <v>63377.587728662831</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
         <f t="shared" ca="1" si="1"/>
-        <v>39768.214914281998</v>
+        <v>40541.83389125923</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
         <f t="shared" ca="1" si="1"/>
-        <v>74753.727715983827</v>
+        <v>70439.37633859145</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113">
         <f t="shared" ca="1" si="1"/>
-        <v>62536.796619170855</v>
+        <v>30931.430268619741</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
         <f t="shared" ca="1" si="1"/>
-        <v>94884.962015393627</v>
+        <v>97193.925668932119</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115">
         <f t="shared" ca="1" si="1"/>
-        <v>28786.31087624899</v>
+        <v>97127.512994646138</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116">
         <f t="shared" ca="1" si="1"/>
-        <v>58589.446770320988</v>
+        <v>50010.894538014538</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117">
         <f t="shared" ca="1" si="1"/>
-        <v>67062.139231929279</v>
+        <v>81621.758979817198</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118">
         <f t="shared" ca="1" si="1"/>
-        <v>21177.100158352856</v>
+        <v>30995.702859997276</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119">
         <f t="shared" ca="1" si="1"/>
-        <v>18103.591898715677</v>
+        <v>62289.688408193666</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120">
         <f t="shared" ca="1" si="1"/>
-        <v>54809.648786970021</v>
+        <v>27064.67872219639</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
         <f t="shared" ca="1" si="1"/>
-        <v>51874.986168305062</v>
+        <v>73098.292556244473</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122">
         <f t="shared" ca="1" si="1"/>
-        <v>4812.3051463622942</v>
+        <v>40560.111859708668</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123">
         <f t="shared" ca="1" si="1"/>
-        <v>373.86943628053837</v>
+        <v>38604.473052597932</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124">
         <f t="shared" ca="1" si="1"/>
-        <v>53590.512425929395</v>
+        <v>76244.452514830933</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125">
         <f t="shared" ca="1" si="1"/>
-        <v>41126.620684124602</v>
+        <v>89284.583988145896</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126">
         <f t="shared" ca="1" si="1"/>
-        <v>49967.798926930518</v>
+        <v>62275.071404995673</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127">
         <f t="shared" ca="1" si="1"/>
-        <v>25876.244899377143</v>
+        <v>83138.117929271975</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128">
         <f t="shared" ca="1" si="1"/>
-        <v>36133.581214444435</v>
+        <v>4331.0540780149513</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129">
         <f t="shared" ca="1" si="1"/>
-        <v>49873.143421257628</v>
+        <v>69644.641777205092</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130">
         <f t="shared" ref="A130:A193" ca="1" si="2">RAND()*100000</f>
-        <v>60302.750395393792</v>
+        <v>25949.08459848223</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131">
         <f t="shared" ca="1" si="2"/>
-        <v>7695.9573429585816</v>
+        <v>48179.118856480753</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132">
         <f t="shared" ca="1" si="2"/>
-        <v>44550.023508455437</v>
+        <v>12573.750247613558</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133">
         <f t="shared" ca="1" si="2"/>
-        <v>96603.503690625163</v>
+        <v>33263.515473833118</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134">
         <f t="shared" ca="1" si="2"/>
-        <v>12968.742056199701</v>
+        <v>9741.7235850954403</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135">
         <f t="shared" ca="1" si="2"/>
-        <v>71863.921733757452</v>
+        <v>49500.175124789537</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136">
         <f t="shared" ca="1" si="2"/>
-        <v>76623.500135806855</v>
+        <v>467.80876597382058</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137">
         <f t="shared" ca="1" si="2"/>
-        <v>85486.713964735434</v>
+        <v>67962.330249025457</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138">
         <f t="shared" ca="1" si="2"/>
-        <v>9196.8241605386629</v>
+        <v>58156.311259642709</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139">
         <f t="shared" ca="1" si="2"/>
-        <v>20767.564577303387</v>
+        <v>72192.094842113889</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140">
         <f t="shared" ca="1" si="2"/>
-        <v>53093.655072953858</v>
+        <v>52660.161801894777</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141">
         <f t="shared" ca="1" si="2"/>
-        <v>40556.606292774944</v>
+        <v>33052.834007310426</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
         <f t="shared" ca="1" si="2"/>
-        <v>13697.036590891754</v>
+        <v>83051.417266437915</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
         <f t="shared" ca="1" si="2"/>
-        <v>21507.664855584862</v>
+        <v>51487.550765243759</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144">
         <f t="shared" ca="1" si="2"/>
-        <v>74707.371475407519</v>
+        <v>39191.456851354444</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145">
         <f t="shared" ca="1" si="2"/>
-        <v>20200.387104787886</v>
+        <v>68800.267647299755</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146">
         <f t="shared" ca="1" si="2"/>
-        <v>38389.962165066507</v>
+        <v>6600.3884360942848</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147">
         <f t="shared" ca="1" si="2"/>
-        <v>72874.970027540025</v>
+        <v>40006.879720447243</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148">
         <f t="shared" ca="1" si="2"/>
-        <v>92409.433429463679</v>
+        <v>95617.390100321092</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
         <f t="shared" ca="1" si="2"/>
-        <v>87459.750590025113</v>
+        <v>44158.778372000692</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150">
         <f t="shared" ca="1" si="2"/>
-        <v>64166.397892656976</v>
+        <v>95058.288421855046</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151">
         <f t="shared" ca="1" si="2"/>
-        <v>31541.408249801992</v>
+        <v>17771.969400563936</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
         <f t="shared" ca="1" si="2"/>
-        <v>58651.81271729849</v>
+        <v>76504.598787671101</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153">
         <f t="shared" ca="1" si="2"/>
-        <v>72220.485870571298</v>
+        <v>78176.664659142931</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
         <f t="shared" ca="1" si="2"/>
-        <v>93591.956893373368</v>
+        <v>92542.17214219259</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155">
         <f t="shared" ca="1" si="2"/>
-        <v>61481.448282826634</v>
+        <v>69235.959600257644</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156">
         <f t="shared" ca="1" si="2"/>
-        <v>92609.437967569014</v>
+        <v>18381.467940397568</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157">
         <f t="shared" ca="1" si="2"/>
-        <v>32890.279451975555</v>
+        <v>85805.0690313011</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158">
         <f t="shared" ca="1" si="2"/>
-        <v>87283.002723791782</v>
+        <v>10624.012731157085</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159">
         <f t="shared" ca="1" si="2"/>
-        <v>86151.906269444837</v>
+        <v>9032.4242683420325</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160">
         <f t="shared" ca="1" si="2"/>
-        <v>28477.864199589818</v>
+        <v>33764.028215368824</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161">
         <f t="shared" ca="1" si="2"/>
-        <v>89583.769756540059</v>
+        <v>40935.276544061126</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162">
         <f t="shared" ca="1" si="2"/>
-        <v>55340.872207003034</v>
+        <v>79450.719435197941</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163">
         <f t="shared" ca="1" si="2"/>
-        <v>16002.960546621725</v>
+        <v>61611.798179132296</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164">
         <f t="shared" ca="1" si="2"/>
-        <v>92525.129075524383</v>
+        <v>24018.152591383845</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165">
         <f t="shared" ca="1" si="2"/>
-        <v>5438.4452602968759</v>
+        <v>71393.250217170193</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166">
         <f t="shared" ca="1" si="2"/>
-        <v>51256.849212885027</v>
+        <v>1832.054180635201</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167">
         <f t="shared" ca="1" si="2"/>
-        <v>94583.754601149078</v>
+        <v>93051.513438975511</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168">
         <f t="shared" ca="1" si="2"/>
-        <v>22776.738249044549</v>
+        <v>11682.136835027834</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169">
         <f t="shared" ca="1" si="2"/>
-        <v>43092.606205815711</v>
+        <v>77490.814139361755</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170">
         <f t="shared" ca="1" si="2"/>
-        <v>60263.337280606698</v>
+        <v>57679.931420812412</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171">
         <f t="shared" ca="1" si="2"/>
-        <v>85900.887913231782</v>
+        <v>38223.692120673601</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
         <f t="shared" ca="1" si="2"/>
-        <v>62994.888765236123</v>
+        <v>3299.8278518536426</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
         <f t="shared" ca="1" si="2"/>
-        <v>61902.248758577407</v>
+        <v>31028.666246120938</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174">
         <f t="shared" ca="1" si="2"/>
-        <v>9883.4346371268311</v>
+        <v>54256.470543713156</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
         <f t="shared" ca="1" si="2"/>
-        <v>85846.743065920644</v>
+        <v>66689.182782969787</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
         <f t="shared" ca="1" si="2"/>
-        <v>49980.0934350362</v>
+        <v>33344.201103018808</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177">
         <f t="shared" ca="1" si="2"/>
-        <v>4356.0117148421114</v>
+        <v>35415.022298921969</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178">
         <f t="shared" ca="1" si="2"/>
-        <v>75855.477215214662</v>
+        <v>50667.74383900666</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179">
         <f t="shared" ca="1" si="2"/>
-        <v>76896.515219393681</v>
+        <v>76630.413958743186</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180">
         <f t="shared" ca="1" si="2"/>
-        <v>8946.6908045144573</v>
+        <v>26984.915530693776</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181">
         <f t="shared" ca="1" si="2"/>
-        <v>23113.771034686757</v>
+        <v>60601.119746843957</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182">
         <f t="shared" ca="1" si="2"/>
-        <v>88477.700029956191</v>
+        <v>36350.201798190807</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183">
         <f t="shared" ca="1" si="2"/>
-        <v>6398.1067734230182</v>
+        <v>84699.813798656833</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184">
         <f t="shared" ca="1" si="2"/>
-        <v>4601.0701622560264</v>
+        <v>94621.378668408594</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185">
         <f t="shared" ca="1" si="2"/>
-        <v>89923.953898012216</v>
+        <v>60973.432750178501</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186">
         <f t="shared" ca="1" si="2"/>
-        <v>12983.686711599707</v>
+        <v>71247.484097857625</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
         <f t="shared" ca="1" si="2"/>
-        <v>75781.601520151075</v>
+        <v>62225.107619030263</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188">
         <f t="shared" ca="1" si="2"/>
-        <v>3021.2764848807415</v>
+        <v>83425.315630866826</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189">
         <f t="shared" ca="1" si="2"/>
-        <v>81822.968694041192</v>
+        <v>37318.595877863314</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190">
         <f t="shared" ca="1" si="2"/>
-        <v>89684.273371997711</v>
+        <v>51716.064632471025</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191">
         <f t="shared" ca="1" si="2"/>
-        <v>79316.98375647144</v>
+        <v>38627.383512473942</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192">
         <f t="shared" ca="1" si="2"/>
-        <v>44497.710615896634</v>
+        <v>26740.60327855765</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
         <f t="shared" ca="1" si="2"/>
-        <v>2980.6494762889879</v>
+        <v>89512.411831032616</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194">
         <f t="shared" ref="A194:A257" ca="1" si="3">RAND()*100000</f>
-        <v>12083.363354043629</v>
+        <v>45960.514143604625</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195">
         <f t="shared" ca="1" si="3"/>
-        <v>49045.075272587521</v>
+        <v>35514.064498636581</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196">
         <f t="shared" ca="1" si="3"/>
-        <v>98137.985427236577</v>
+        <v>40465.296340072979</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197">
         <f t="shared" ca="1" si="3"/>
-        <v>75754.0341636175</v>
+        <v>13991.336955448896</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198">
         <f t="shared" ca="1" si="3"/>
-        <v>41774.957254783454</v>
+        <v>26881.606679365399</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199">
         <f t="shared" ca="1" si="3"/>
-        <v>46977.545265156754</v>
+        <v>38535.960809503304</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200">
         <f t="shared" ca="1" si="3"/>
-        <v>38187.965398813947</v>
+        <v>81416.784232207778</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
         <f t="shared" ca="1" si="3"/>
-        <v>39680.92469686336</v>
+        <v>22566.01170973913</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
         <f t="shared" ca="1" si="3"/>
-        <v>29659.242876973589</v>
+        <v>78824.723536430232</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
         <f t="shared" ca="1" si="3"/>
-        <v>46118.783701005108</v>
+        <v>3023.4531036890776</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204">
         <f t="shared" ca="1" si="3"/>
-        <v>92555.663755051311</v>
+        <v>24414.631168144551</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205">
         <f t="shared" ca="1" si="3"/>
-        <v>40086.141610395185</v>
+        <v>27145.979117462924</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
         <f t="shared" ca="1" si="3"/>
-        <v>86752.268197636746</v>
+        <v>18273.389911930248</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
         <f t="shared" ca="1" si="3"/>
-        <v>78430.686861620299</v>
+        <v>5578.8316805666091</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
         <f t="shared" ca="1" si="3"/>
-        <v>90248.136199847067</v>
+        <v>36982.342967789431</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
         <f t="shared" ca="1" si="3"/>
-        <v>54454.941956314738</v>
+        <v>28572.761662181212</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210">
         <f t="shared" ca="1" si="3"/>
-        <v>34884.868167226676</v>
+        <v>11840.009504152793</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211">
         <f t="shared" ca="1" si="3"/>
-        <v>59725.682241492432</v>
+        <v>84237.571619156748</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212">
         <f t="shared" ca="1" si="3"/>
-        <v>94192.84652991344</v>
+        <v>41770.958510871169</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213">
         <f t="shared" ca="1" si="3"/>
-        <v>79014.191711972497</v>
+        <v>87628.692349672579</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214">
         <f t="shared" ca="1" si="3"/>
-        <v>76331.985251478705</v>
+        <v>75312.445945686733</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215">
         <f t="shared" ca="1" si="3"/>
-        <v>66602.007959066003</v>
+        <v>72469.301476151304</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
         <f t="shared" ca="1" si="3"/>
-        <v>91836.828251356172</v>
+        <v>34862.187741981463</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217">
         <f t="shared" ca="1" si="3"/>
-        <v>13571.246099444123</v>
+        <v>29020.842116021529</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218">
         <f t="shared" ca="1" si="3"/>
-        <v>2363.531315315015</v>
+        <v>75964.169869975085</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219">
         <f t="shared" ca="1" si="3"/>
-        <v>95945.021784408964</v>
+        <v>20322.967443154415</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220">
         <f t="shared" ca="1" si="3"/>
-        <v>39134.434526571436</v>
+        <v>89349.404804427482</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221">
         <f t="shared" ca="1" si="3"/>
-        <v>25703.13155399332</v>
+        <v>37038.66404681807</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
         <f t="shared" ca="1" si="3"/>
-        <v>54672.462694627058</v>
+        <v>78070.346916119714</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
         <f t="shared" ca="1" si="3"/>
-        <v>84964.947232444756</v>
+        <v>47358.029047375741</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224">
         <f t="shared" ca="1" si="3"/>
-        <v>571.59372350064075</v>
+        <v>91008.260179235818</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225">
         <f t="shared" ca="1" si="3"/>
-        <v>98526.331807917246</v>
+        <v>34248.440875490218</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226">
         <f t="shared" ca="1" si="3"/>
-        <v>73374.470024621798</v>
+        <v>10391.322549545401</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227">
         <f t="shared" ca="1" si="3"/>
-        <v>20525.729358891385</v>
+        <v>42749.627284016293</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228">
         <f t="shared" ca="1" si="3"/>
-        <v>48004.495571533669</v>
+        <v>96650.110866667703</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229">
         <f t="shared" ca="1" si="3"/>
-        <v>88994.487159969285</v>
+        <v>8327.767311707179</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230">
         <f t="shared" ca="1" si="3"/>
-        <v>51804.457585305827</v>
+        <v>5781.1773768037474</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
         <f t="shared" ca="1" si="3"/>
-        <v>83342.186647523369</v>
+        <v>56904.203721400358</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232">
         <f t="shared" ca="1" si="3"/>
-        <v>64097.901269060596</v>
+        <v>31620.426030182436</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233">
         <f t="shared" ca="1" si="3"/>
-        <v>76153.229999065603</v>
+        <v>94595.453189895779</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234">
         <f t="shared" ca="1" si="3"/>
-        <v>94186.138727046302</v>
+        <v>51646.094319921176</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235">
         <f t="shared" ca="1" si="3"/>
-        <v>54346.570956336203</v>
+        <v>1768.1663188027774</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
         <f t="shared" ca="1" si="3"/>
-        <v>39761.415176657465</v>
+        <v>78182.611156409956</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
         <f t="shared" ca="1" si="3"/>
-        <v>74217.244850070114</v>
+        <v>99107.82458367759</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238">
         <f t="shared" ca="1" si="3"/>
-        <v>41272.411263498798</v>
+        <v>16701.102356757347</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239">
         <f t="shared" ca="1" si="3"/>
-        <v>28473.226816118302</v>
+        <v>39565.727645574312</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240">
         <f t="shared" ca="1" si="3"/>
-        <v>53678.101606218057</v>
+        <v>68793.574687185872</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241">
         <f t="shared" ca="1" si="3"/>
-        <v>63617.885943542598</v>
+        <v>74843.116358003404</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242">
         <f t="shared" ca="1" si="3"/>
-        <v>7132.4136686958473</v>
+        <v>15366.027291934537</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243">
         <f t="shared" ca="1" si="3"/>
-        <v>86381.533634828127</v>
+        <v>52394.672163811272</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244">
         <f t="shared" ca="1" si="3"/>
-        <v>39544.914957751607</v>
+        <v>18291.312478934229</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245">
         <f t="shared" ca="1" si="3"/>
-        <v>95336.422265699744</v>
+        <v>58214.513571275093</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246">
         <f t="shared" ca="1" si="3"/>
-        <v>6602.1728815356282</v>
+        <v>69399.707790619927</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247">
         <f t="shared" ca="1" si="3"/>
-        <v>44951.51528852238</v>
+        <v>36017.455928683383</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248">
         <f t="shared" ca="1" si="3"/>
-        <v>6970.5525913967722</v>
+        <v>70603.515212142171</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249">
         <f t="shared" ca="1" si="3"/>
-        <v>41156.973593874303</v>
+        <v>83301.670827587528</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250">
         <f t="shared" ca="1" si="3"/>
-        <v>69137.328662142245</v>
+        <v>45464.633406604269</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
         <f t="shared" ca="1" si="3"/>
-        <v>70194.469564775995</v>
+        <v>15676.500701470164</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252">
         <f t="shared" ca="1" si="3"/>
-        <v>80886.944568909908</v>
+        <v>7651.5012221169409</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253">
         <f t="shared" ca="1" si="3"/>
-        <v>4685.809718110645</v>
+        <v>65397.391347183373</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254">
         <f t="shared" ca="1" si="3"/>
-        <v>88396.367422722702</v>
+        <v>8531.8709007869747</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
         <f t="shared" ca="1" si="3"/>
-        <v>80617.598706013858</v>
+        <v>72731.049191595404</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
         <f t="shared" ca="1" si="3"/>
-        <v>92013.991781264704</v>
+        <v>64874.600947967352</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257">
         <f t="shared" ca="1" si="3"/>
-        <v>34814.992217489795</v>
+        <v>15.901810169416386</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258">
         <f t="shared" ref="A258:A300" ca="1" si="4">RAND()*100000</f>
-        <v>28097.385175128766</v>
+        <v>10228.309508498123</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259">
         <f t="shared" ca="1" si="4"/>
-        <v>22589.804452658846</v>
+        <v>24046.794999486065</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260">
         <f t="shared" ca="1" si="4"/>
-        <v>8003.9267387630671</v>
+        <v>28483.625607337613</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
         <f t="shared" ca="1" si="4"/>
-        <v>85431.506960941348</v>
+        <v>95204.519168153463</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262">
         <f t="shared" ca="1" si="4"/>
-        <v>75508.005758443382</v>
+        <v>69320.856995725611</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263">
         <f t="shared" ca="1" si="4"/>
-        <v>14481.367033972114</v>
+        <v>44602.21128073553</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264">
         <f t="shared" ca="1" si="4"/>
-        <v>85389.153578363912</v>
+        <v>79853.902242130265</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265">
         <f t="shared" ca="1" si="4"/>
-        <v>79856.935646079131</v>
+        <v>72422.298605584714</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
         <f t="shared" ca="1" si="4"/>
-        <v>54004.088518956072</v>
+        <v>17096.775239440078</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
         <f t="shared" ca="1" si="4"/>
-        <v>70303.100109530133</v>
+        <v>29929.896297315041</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268">
         <f t="shared" ca="1" si="4"/>
-        <v>18340.859484634919</v>
+        <v>70043.668884075669</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269">
         <f t="shared" ca="1" si="4"/>
-        <v>64671.886578125515</v>
+        <v>17930.230288650197</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270">
         <f t="shared" ca="1" si="4"/>
-        <v>93436.334670170341</v>
+        <v>60054.78516299653</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271">
         <f t="shared" ca="1" si="4"/>
-        <v>65501.793511033349</v>
+        <v>71699.901905679522</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272">
         <f t="shared" ca="1" si="4"/>
-        <v>70829.847146899876</v>
+        <v>30170.808449772147</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273">
         <f t="shared" ca="1" si="4"/>
-        <v>58894.097453632909</v>
+        <v>14397.100696723397</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274">
         <f t="shared" ca="1" si="4"/>
-        <v>83271.295878935314</v>
+        <v>71992.817062586328</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275">
         <f t="shared" ca="1" si="4"/>
-        <v>40037.115516413745</v>
+        <v>91457.762100406355</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276">
         <f t="shared" ca="1" si="4"/>
-        <v>88014.087011357726</v>
+        <v>71204.748462512274</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277">
         <f t="shared" ca="1" si="4"/>
-        <v>85601.407136190741</v>
+        <v>45730.297720649083</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278">
         <f t="shared" ca="1" si="4"/>
-        <v>71542.35573852199</v>
+        <v>18499.706973085518</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279">
         <f t="shared" ca="1" si="4"/>
-        <v>84397.463937611727</v>
+        <v>10389.546592684195</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
         <f t="shared" ca="1" si="4"/>
-        <v>16357.583194433346</v>
+        <v>81377.008333926322</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281">
         <f t="shared" ca="1" si="4"/>
-        <v>4814.6727233591037</v>
+        <v>90536.97944717131</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282">
         <f t="shared" ca="1" si="4"/>
-        <v>95630.84066112338</v>
+        <v>67819.672959943447</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283">
         <f t="shared" ca="1" si="4"/>
-        <v>91995.919564788346</v>
+        <v>92036.07287266913</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284">
         <f t="shared" ca="1" si="4"/>
-        <v>33949.666348822735</v>
+        <v>90669.473174285115</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285">
         <f t="shared" ca="1" si="4"/>
-        <v>86179.869146725367</v>
+        <v>64540.086198993784</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286">
         <f t="shared" ca="1" si="4"/>
-        <v>70228.983650035108</v>
+        <v>73315.389432455006</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287">
         <f t="shared" ca="1" si="4"/>
-        <v>49754.894864872098</v>
+        <v>94645.400258642854</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288">
         <f t="shared" ca="1" si="4"/>
-        <v>23460.432086413784</v>
+        <v>63536.155901395905</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289">
         <f t="shared" ca="1" si="4"/>
-        <v>84523.948422995178</v>
+        <v>79912.684502529082</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290">
         <f t="shared" ca="1" si="4"/>
-        <v>80153.255715943596</v>
+        <v>8286.1683182109409</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291">
         <f t="shared" ca="1" si="4"/>
-        <v>63822.681763306318</v>
+        <v>80670.439811768738</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292">
         <f t="shared" ca="1" si="4"/>
-        <v>19369.125881710315</v>
+        <v>46737.69612177994</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293">
         <f t="shared" ca="1" si="4"/>
-        <v>5413.5057739180929</v>
+        <v>70055.198335036461</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294">
         <f t="shared" ca="1" si="4"/>
-        <v>24042.548940684661</v>
+        <v>79820.626930112368</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295">
         <f t="shared" ca="1" si="4"/>
-        <v>34339.234338081849</v>
+        <v>6226.3033051919938</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296">
         <f t="shared" ca="1" si="4"/>
-        <v>11160.058858912169</v>
+        <v>90676.871915279684</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297">
         <f t="shared" ca="1" si="4"/>
-        <v>20161.795299936726</v>
+        <v>46780.617784303766</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298">
         <f t="shared" ca="1" si="4"/>
-        <v>21487.609872025172</v>
+        <v>17451.705751560832</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299">
         <f t="shared" ca="1" si="4"/>
-        <v>4756.5695985060001</v>
+        <v>21577.285602024287</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300">
         <f t="shared" ca="1" si="4"/>
-        <v>34784.457750445566</v>
+        <v>40675.788733122361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>